<commit_message>
broken version do not use
</commit_message>
<xml_diff>
--- a/target debugger.xlsx
+++ b/target debugger.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\keegan\Downloads\A6Start\A6Start\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{11E05D7C-7AE5-4B5B-BFD5-F2A5ECB948E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79DA0655-F249-4DBD-94A3-768B789517A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{D1BDAA98-E73A-46CB-A5CF-2E613F0DCE3E}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="581" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="579" uniqueCount="139">
   <si>
     <t>x</t>
   </si>
@@ -77,9 +77,6 @@
     <t>[x=4,y=2]</t>
   </si>
   <si>
-    <t>[x=0,y=13]</t>
-  </si>
-  <si>
     <t>[x=3,y=9]</t>
   </si>
   <si>
@@ -200,9 +197,6 @@
     <t>[x=1,y=7]</t>
   </si>
   <si>
-    <t>[x=0,y=11]</t>
-  </si>
-  <si>
     <t>[x=1,y=5]</t>
   </si>
   <si>
@@ -368,9 +362,6 @@
     <t>[x=3,y=0]</t>
   </si>
   <si>
-    <t>[x=2,y=13]</t>
-  </si>
-  <si>
     <t>[x=1,y=6]</t>
   </si>
   <si>
@@ -459,6 +450,9 @@
   </si>
   <si>
     <t>put hits here</t>
+  </si>
+  <si>
+    <t>[x=1,y=0]</t>
   </si>
 </sst>
 </file>
@@ -950,7 +944,7 @@
   <dimension ref="A1:AD389"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AB14" sqref="AB14"/>
+      <selection activeCell="Q9" sqref="Q9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -962,26 +956,26 @@
   <sheetData>
     <row r="1" spans="1:30">
       <c r="R1" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="S1">
         <f>COUNTA(U:U) -1</f>
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="U1" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="AB1" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
     </row>
     <row r="2" spans="1:30">
       <c r="R2" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="S2" s="2">
         <f>S1/(15*15)</f>
-        <v>0.6</v>
+        <v>0.59111111111111114</v>
       </c>
     </row>
     <row r="5" spans="1:30">
@@ -1040,7 +1034,7 @@
         <v>7</v>
       </c>
       <c r="AD5" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="6" spans="1:30">
@@ -1054,7 +1048,7 @@
       </c>
       <c r="C6" t="str">
         <f t="shared" ref="C6:P20" si="0">_xlfn.XLOOKUP("[x="&amp;C$5&amp;",y="&amp;$A6&amp;"]",$AB:$AB,$AD:$AD,_xlfn.XLOOKUP("[x="&amp;C$5&amp;",y="&amp;$A6&amp;"]",$U:$U,$Y:$Y,"o"))</f>
-        <v>o</v>
+        <v>x</v>
       </c>
       <c r="D6" t="str">
         <f t="shared" si="0"/>
@@ -1115,10 +1109,10 @@
         <v>0</v>
       </c>
       <c r="AB6" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="AD6" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="7" spans="1:30">
@@ -1187,16 +1181,16 @@
         <v>o</v>
       </c>
       <c r="U7" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="Y7" t="s">
         <v>0</v>
       </c>
       <c r="AB7" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AD7" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="8" spans="1:30">
@@ -1229,7 +1223,7 @@
         <v>P</v>
       </c>
       <c r="H8" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.XLOOKUP("[x="&amp;H$5&amp;",y="&amp;$A8&amp;"]",$AB:$AB,$AD:$AD,_xlfn.XLOOKUP("[x="&amp;H$5&amp;",y="&amp;$A8&amp;"]",$U:$U,$Y:$Y,"o"))</f>
         <v>P</v>
       </c>
       <c r="I8" t="str">
@@ -1271,10 +1265,10 @@
         <v>0</v>
       </c>
       <c r="AB8" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="AD8" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="9" spans="1:30">
@@ -1349,10 +1343,10 @@
         <v>0</v>
       </c>
       <c r="AB9" s="1" t="s">
-        <v>80</v>
+        <v>95</v>
       </c>
       <c r="AD9" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="10" spans="1:30">
@@ -1421,16 +1415,16 @@
         <v>o</v>
       </c>
       <c r="U10" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="Y10" t="s">
         <v>0</v>
       </c>
       <c r="AB10" s="1" t="s">
-        <v>95</v>
+        <v>78</v>
       </c>
       <c r="AD10" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="11" spans="1:30">
@@ -1505,10 +1499,10 @@
         <v>0</v>
       </c>
       <c r="AB11" s="1" t="s">
-        <v>41</v>
+        <v>93</v>
       </c>
       <c r="AD11" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="12" spans="1:30">
@@ -1583,10 +1577,10 @@
         <v>0</v>
       </c>
       <c r="AB12" s="1" t="s">
-        <v>96</v>
+        <v>40</v>
       </c>
       <c r="AD12" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="13" spans="1:30">
@@ -1655,16 +1649,16 @@
         <v>o</v>
       </c>
       <c r="U13" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="Y13" t="s">
         <v>0</v>
       </c>
       <c r="AB13" s="1" t="s">
-        <v>77</v>
+        <v>94</v>
       </c>
       <c r="AD13" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="14" spans="1:30">
@@ -1733,16 +1727,16 @@
         <v>o</v>
       </c>
       <c r="U14" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="Y14" t="s">
         <v>0</v>
       </c>
       <c r="AB14" s="1" t="s">
-        <v>97</v>
+        <v>75</v>
       </c>
       <c r="AD14" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="15" spans="1:30">
@@ -1820,7 +1814,7 @@
         <v>12</v>
       </c>
       <c r="AD15" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="16" spans="1:30">
@@ -1889,16 +1883,16 @@
         <v>o</v>
       </c>
       <c r="U16" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="Y16" t="s">
         <v>0</v>
       </c>
       <c r="AB16" s="1" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="AD16" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="17" spans="1:30">
@@ -1908,7 +1902,7 @@
       </c>
       <c r="B17" t="str">
         <f t="shared" si="1"/>
-        <v>x</v>
+        <v>o</v>
       </c>
       <c r="C17" t="str">
         <f t="shared" si="0"/>
@@ -1967,16 +1961,16 @@
         <v>o</v>
       </c>
       <c r="U17" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="Y17" t="s">
         <v>0</v>
       </c>
       <c r="AB17" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="AD17" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="18" spans="1:30">
@@ -2045,16 +2039,16 @@
         <v>x</v>
       </c>
       <c r="U18" s="1" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="Y18" t="s">
         <v>0</v>
       </c>
       <c r="AB18" s="1" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="AD18" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="19" spans="1:30">
@@ -2064,7 +2058,7 @@
       </c>
       <c r="B19" t="str">
         <f t="shared" si="1"/>
-        <v>x</v>
+        <v>o</v>
       </c>
       <c r="C19" t="str">
         <f t="shared" si="0"/>
@@ -2072,7 +2066,7 @@
       </c>
       <c r="D19" t="str">
         <f t="shared" si="0"/>
-        <v>x</v>
+        <v>o</v>
       </c>
       <c r="E19" t="str">
         <f t="shared" si="0"/>
@@ -2129,10 +2123,10 @@
         <v>0</v>
       </c>
       <c r="AB19" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="AD19" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="20" spans="1:30">
@@ -2207,10 +2201,10 @@
         <v>0</v>
       </c>
       <c r="AB20" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="AD20" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="21" spans="1:30">
@@ -2221,24 +2215,24 @@
         <v>0</v>
       </c>
       <c r="AB21" s="1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="AD21" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="22" spans="1:30">
       <c r="U22" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="Y22" t="s">
         <v>0</v>
       </c>
       <c r="AB22" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="AD22" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="23" spans="1:30">
@@ -2249,10 +2243,10 @@
         <v>0</v>
       </c>
       <c r="AB23" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="AD23" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="24" spans="1:30">
@@ -2263,52 +2257,52 @@
         <v>0</v>
       </c>
       <c r="AB24" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="AD24" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="25" spans="1:30">
       <c r="U25" s="1" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="Y25" t="s">
         <v>0</v>
       </c>
       <c r="AB25" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="AD25" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="26" spans="1:30">
       <c r="U26" s="1" t="s">
-        <v>110</v>
+        <v>13</v>
       </c>
       <c r="Y26" t="s">
         <v>0</v>
       </c>
       <c r="AB26" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AD26" t="s">
         <v>102</v>
-      </c>
-      <c r="AD26" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="27" spans="1:30">
       <c r="U27" s="1" t="s">
-        <v>13</v>
+        <v>108</v>
       </c>
       <c r="Y27" t="s">
         <v>0</v>
       </c>
       <c r="AB27" s="1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="AD27" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="28" spans="1:30">
@@ -2319,21 +2313,21 @@
         <v>0</v>
       </c>
       <c r="AB28" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="AD28" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="29" spans="1:30">
       <c r="U29" s="1" t="s">
-        <v>111</v>
+        <v>16</v>
       </c>
       <c r="Y29" t="s">
         <v>0</v>
       </c>
       <c r="AD29" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="30" spans="1:30">
@@ -2344,89 +2338,89 @@
         <v>0</v>
       </c>
       <c r="AD30" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="31" spans="1:30">
       <c r="U31" s="1" t="s">
-        <v>17</v>
+        <v>97</v>
       </c>
       <c r="Y31" t="s">
         <v>0</v>
       </c>
       <c r="AD31" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="32" spans="1:30">
       <c r="U32" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="Y32" t="s">
         <v>0</v>
       </c>
       <c r="AD32" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="33" spans="21:30">
       <c r="U33" s="1" t="s">
-        <v>99</v>
+        <v>17</v>
       </c>
       <c r="Y33" t="s">
         <v>0</v>
       </c>
       <c r="AD33" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="34" spans="21:30">
       <c r="U34" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="Y34" t="s">
         <v>0</v>
       </c>
       <c r="AD34" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="35" spans="21:30">
       <c r="U35" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="Y35" t="s">
         <v>0</v>
       </c>
       <c r="AD35" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="36" spans="21:30">
       <c r="U36" s="1" t="s">
-        <v>21</v>
+        <v>109</v>
       </c>
       <c r="Y36" t="s">
         <v>0</v>
       </c>
       <c r="AD36" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="37" spans="21:30">
       <c r="U37" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="Y37" t="s">
         <v>0</v>
       </c>
       <c r="AD37" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="38" spans="21:30">
       <c r="U38" s="1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="Y38" t="s">
         <v>0</v>
@@ -2434,7 +2428,7 @@
     </row>
     <row r="39" spans="21:30">
       <c r="U39" s="1" t="s">
-        <v>22</v>
+        <v>94</v>
       </c>
       <c r="Y39" t="s">
         <v>0</v>
@@ -2442,7 +2436,7 @@
     </row>
     <row r="40" spans="21:30">
       <c r="U40" s="1" t="s">
-        <v>113</v>
+        <v>22</v>
       </c>
       <c r="Y40" t="s">
         <v>0</v>
@@ -2450,7 +2444,7 @@
     </row>
     <row r="41" spans="21:30">
       <c r="U41" s="1" t="s">
-        <v>96</v>
+        <v>23</v>
       </c>
       <c r="Y41" t="s">
         <v>0</v>
@@ -2458,7 +2452,7 @@
     </row>
     <row r="42" spans="21:30">
       <c r="U42" s="1" t="s">
-        <v>23</v>
+        <v>111</v>
       </c>
       <c r="Y42" t="s">
         <v>0</v>
@@ -2474,7 +2468,7 @@
     </row>
     <row r="44" spans="21:30">
       <c r="U44" s="1" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="Y44" t="s">
         <v>0</v>
@@ -2490,7 +2484,7 @@
     </row>
     <row r="46" spans="21:30">
       <c r="U46" s="1" t="s">
-        <v>115</v>
+        <v>26</v>
       </c>
       <c r="Y46" t="s">
         <v>0</v>
@@ -2498,7 +2492,7 @@
     </row>
     <row r="47" spans="21:30">
       <c r="U47" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="Y47" t="s">
         <v>0</v>
@@ -2506,7 +2500,7 @@
     </row>
     <row r="48" spans="21:30">
       <c r="U48" s="1" t="s">
-        <v>27</v>
+        <v>113</v>
       </c>
       <c r="Y48" t="s">
         <v>0</v>
@@ -2514,7 +2508,7 @@
     </row>
     <row r="49" spans="21:25">
       <c r="U49" s="1" t="s">
-        <v>28</v>
+        <v>99</v>
       </c>
       <c r="Y49" t="s">
         <v>0</v>
@@ -2522,7 +2516,7 @@
     </row>
     <row r="50" spans="21:25">
       <c r="U50" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="Y50" t="s">
         <v>0</v>
@@ -2530,7 +2524,7 @@
     </row>
     <row r="51" spans="21:25">
       <c r="U51" s="1" t="s">
-        <v>101</v>
+        <v>28</v>
       </c>
       <c r="Y51" t="s">
         <v>0</v>
@@ -2538,7 +2532,7 @@
     </row>
     <row r="52" spans="21:25">
       <c r="U52" s="1" t="s">
-        <v>117</v>
+        <v>29</v>
       </c>
       <c r="Y52" t="s">
         <v>0</v>
@@ -2546,7 +2540,7 @@
     </row>
     <row r="53" spans="21:25">
       <c r="U53" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="Y53" t="s">
         <v>0</v>
@@ -2554,7 +2548,7 @@
     </row>
     <row r="54" spans="21:25">
       <c r="U54" s="1" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="Y54" t="s">
         <v>0</v>
@@ -2578,7 +2572,7 @@
     </row>
     <row r="57" spans="21:25">
       <c r="U57" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="Y57" t="s">
         <v>0</v>
@@ -2586,7 +2580,7 @@
     </row>
     <row r="58" spans="21:25">
       <c r="U58" s="1" t="s">
-        <v>34</v>
+        <v>115</v>
       </c>
       <c r="Y58" t="s">
         <v>0</v>
@@ -2594,7 +2588,7 @@
     </row>
     <row r="59" spans="21:25">
       <c r="U59" s="1" t="s">
-        <v>35</v>
+        <v>116</v>
       </c>
       <c r="Y59" t="s">
         <v>0</v>
@@ -2602,7 +2596,7 @@
     </row>
     <row r="60" spans="21:25">
       <c r="U60" s="1" t="s">
-        <v>118</v>
+        <v>35</v>
       </c>
       <c r="Y60" t="s">
         <v>0</v>
@@ -2610,7 +2604,7 @@
     </row>
     <row r="61" spans="21:25">
       <c r="U61" s="1" t="s">
-        <v>119</v>
+        <v>36</v>
       </c>
       <c r="Y61" t="s">
         <v>0</v>
@@ -2618,7 +2612,7 @@
     </row>
     <row r="62" spans="21:25">
       <c r="U62" s="1" t="s">
-        <v>36</v>
+        <v>117</v>
       </c>
       <c r="Y62" t="s">
         <v>0</v>
@@ -2634,7 +2628,7 @@
     </row>
     <row r="64" spans="21:25">
       <c r="U64" s="1" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="Y64" t="s">
         <v>0</v>
@@ -2650,7 +2644,7 @@
     </row>
     <row r="66" spans="21:25">
       <c r="U66" s="1" t="s">
-        <v>121</v>
+        <v>39</v>
       </c>
       <c r="Y66" t="s">
         <v>0</v>
@@ -2658,7 +2652,7 @@
     </row>
     <row r="67" spans="21:25">
       <c r="U67" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="Y67" t="s">
         <v>0</v>
@@ -2666,7 +2660,7 @@
     </row>
     <row r="68" spans="21:25">
       <c r="U68" s="1" t="s">
-        <v>40</v>
+        <v>119</v>
       </c>
       <c r="Y68" t="s">
         <v>0</v>
@@ -2682,7 +2676,7 @@
     </row>
     <row r="70" spans="21:25">
       <c r="U70" s="1" t="s">
-        <v>122</v>
+        <v>42</v>
       </c>
       <c r="Y70" t="s">
         <v>0</v>
@@ -2690,7 +2684,7 @@
     </row>
     <row r="71" spans="21:25">
       <c r="U71" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="Y71" t="s">
         <v>0</v>
@@ -2698,7 +2692,7 @@
     </row>
     <row r="72" spans="21:25">
       <c r="U72" s="1" t="s">
-        <v>43</v>
+        <v>120</v>
       </c>
       <c r="Y72" t="s">
         <v>0</v>
@@ -2714,7 +2708,7 @@
     </row>
     <row r="74" spans="21:25">
       <c r="U74" s="1" t="s">
-        <v>123</v>
+        <v>45</v>
       </c>
       <c r="Y74" t="s">
         <v>0</v>
@@ -2722,7 +2716,7 @@
     </row>
     <row r="75" spans="21:25">
       <c r="U75" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="Y75" t="s">
         <v>0</v>
@@ -2730,7 +2724,7 @@
     </row>
     <row r="76" spans="21:25">
       <c r="U76" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="Y76" t="s">
         <v>0</v>
@@ -2738,7 +2732,7 @@
     </row>
     <row r="77" spans="21:25">
       <c r="U77" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="Y77" t="s">
         <v>0</v>
@@ -2746,7 +2740,7 @@
     </row>
     <row r="78" spans="21:25">
       <c r="U78" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="Y78" t="s">
         <v>0</v>
@@ -2754,7 +2748,7 @@
     </row>
     <row r="79" spans="21:25">
       <c r="U79" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="Y79" t="s">
         <v>0</v>
@@ -2762,7 +2756,7 @@
     </row>
     <row r="80" spans="21:25">
       <c r="U80" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="Y80" t="s">
         <v>0</v>
@@ -2770,7 +2764,7 @@
     </row>
     <row r="81" spans="21:25">
       <c r="U81" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="Y81" t="s">
         <v>0</v>
@@ -2778,7 +2772,7 @@
     </row>
     <row r="82" spans="21:25">
       <c r="U82" s="1" t="s">
-        <v>52</v>
+        <v>121</v>
       </c>
       <c r="Y82" t="s">
         <v>0</v>
@@ -2794,7 +2788,7 @@
     </row>
     <row r="84" spans="21:25">
       <c r="U84" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="Y84" t="s">
         <v>0</v>
@@ -2802,7 +2796,7 @@
     </row>
     <row r="85" spans="21:25">
       <c r="U85" s="1" t="s">
-        <v>54</v>
+        <v>93</v>
       </c>
       <c r="Y85" t="s">
         <v>0</v>
@@ -2810,7 +2804,7 @@
     </row>
     <row r="86" spans="21:25">
       <c r="U86" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="Y86" t="s">
         <v>0</v>
@@ -2818,7 +2812,7 @@
     </row>
     <row r="87" spans="21:25">
       <c r="U87" s="1" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="Y87" t="s">
         <v>0</v>
@@ -2826,7 +2820,7 @@
     </row>
     <row r="88" spans="21:25">
       <c r="U88" s="1" t="s">
-        <v>95</v>
+        <v>124</v>
       </c>
       <c r="Y88" t="s">
         <v>0</v>
@@ -2834,7 +2828,7 @@
     </row>
     <row r="89" spans="21:25">
       <c r="U89" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="Y89" t="s">
         <v>0</v>
@@ -2842,7 +2836,7 @@
     </row>
     <row r="90" spans="21:25">
       <c r="U90" s="1" t="s">
-        <v>126</v>
+        <v>56</v>
       </c>
       <c r="Y90" t="s">
         <v>0</v>
@@ -2850,7 +2844,7 @@
     </row>
     <row r="91" spans="21:25">
       <c r="U91" s="1" t="s">
-        <v>127</v>
+        <v>57</v>
       </c>
       <c r="Y91" t="s">
         <v>0</v>
@@ -2858,7 +2852,7 @@
     </row>
     <row r="92" spans="21:25">
       <c r="U92" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="Y92" t="s">
         <v>0</v>
@@ -2866,7 +2860,7 @@
     </row>
     <row r="93" spans="21:25">
       <c r="U93" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="Y93" t="s">
         <v>0</v>
@@ -2874,7 +2868,7 @@
     </row>
     <row r="94" spans="21:25">
       <c r="U94" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="Y94" t="s">
         <v>0</v>
@@ -2882,7 +2876,7 @@
     </row>
     <row r="95" spans="21:25">
       <c r="U95" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="Y95" t="s">
         <v>0</v>
@@ -2890,7 +2884,7 @@
     </row>
     <row r="96" spans="21:25">
       <c r="U96" s="1" t="s">
-        <v>61</v>
+        <v>125</v>
       </c>
       <c r="Y96" t="s">
         <v>0</v>
@@ -2906,7 +2900,7 @@
     </row>
     <row r="98" spans="21:25">
       <c r="U98" s="1" t="s">
-        <v>63</v>
+        <v>126</v>
       </c>
       <c r="Y98" t="s">
         <v>0</v>
@@ -2914,7 +2908,7 @@
     </row>
     <row r="99" spans="21:25">
       <c r="U99" s="1" t="s">
-        <v>128</v>
+        <v>64</v>
       </c>
       <c r="Y99" t="s">
         <v>0</v>
@@ -2922,7 +2916,7 @@
     </row>
     <row r="100" spans="21:25">
       <c r="U100" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="Y100" t="s">
         <v>0</v>
@@ -2930,7 +2924,7 @@
     </row>
     <row r="101" spans="21:25">
       <c r="U101" s="1" t="s">
-        <v>129</v>
+        <v>65</v>
       </c>
       <c r="Y101" t="s">
         <v>0</v>
@@ -2938,7 +2932,7 @@
     </row>
     <row r="102" spans="21:25">
       <c r="U102" s="1" t="s">
-        <v>66</v>
+        <v>127</v>
       </c>
       <c r="Y102" t="s">
         <v>0</v>
@@ -2946,7 +2940,7 @@
     </row>
     <row r="103" spans="21:25">
       <c r="U103" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="Y103" t="s">
         <v>0</v>
@@ -2962,7 +2956,7 @@
     </row>
     <row r="105" spans="21:25">
       <c r="U105" s="1" t="s">
-        <v>130</v>
+        <v>68</v>
       </c>
       <c r="Y105" t="s">
         <v>0</v>
@@ -2970,7 +2964,7 @@
     </row>
     <row r="106" spans="21:25">
       <c r="U106" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="Y106" t="s">
         <v>0</v>
@@ -2978,7 +2972,7 @@
     </row>
     <row r="107" spans="21:25">
       <c r="U107" s="1" t="s">
-        <v>69</v>
+        <v>128</v>
       </c>
       <c r="Y107" t="s">
         <v>0</v>
@@ -3002,7 +2996,7 @@
     </row>
     <row r="110" spans="21:25">
       <c r="U110" s="1" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="Y110" t="s">
         <v>0</v>
@@ -3010,7 +3004,7 @@
     </row>
     <row r="111" spans="21:25">
       <c r="U111" s="1" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="Y111" t="s">
         <v>0</v>
@@ -3018,7 +3012,7 @@
     </row>
     <row r="112" spans="21:25">
       <c r="U112" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="Y112" t="s">
         <v>0</v>
@@ -3026,7 +3020,7 @@
     </row>
     <row r="113" spans="21:25">
       <c r="U113" s="1" t="s">
-        <v>132</v>
+        <v>74</v>
       </c>
       <c r="Y113" t="s">
         <v>0</v>
@@ -3042,7 +3036,7 @@
     </row>
     <row r="115" spans="21:25">
       <c r="U115" s="1" t="s">
-        <v>74</v>
+        <v>130</v>
       </c>
       <c r="Y115" t="s">
         <v>0</v>
@@ -3058,7 +3052,7 @@
     </row>
     <row r="117" spans="21:25">
       <c r="U117" s="1" t="s">
-        <v>77</v>
+        <v>131</v>
       </c>
       <c r="Y117" t="s">
         <v>0</v>
@@ -3066,7 +3060,7 @@
     </row>
     <row r="118" spans="21:25">
       <c r="U118" s="1" t="s">
-        <v>133</v>
+        <v>77</v>
       </c>
       <c r="Y118" t="s">
         <v>0</v>
@@ -3074,7 +3068,7 @@
     </row>
     <row r="119" spans="21:25">
       <c r="U119" s="1" t="s">
-        <v>78</v>
+        <v>132</v>
       </c>
       <c r="Y119" t="s">
         <v>0</v>
@@ -3082,7 +3076,7 @@
     </row>
     <row r="120" spans="21:25">
       <c r="U120" s="1" t="s">
-        <v>134</v>
+        <v>78</v>
       </c>
       <c r="Y120" t="s">
         <v>0</v>
@@ -3098,7 +3092,7 @@
     </row>
     <row r="122" spans="21:25">
       <c r="U122" s="1" t="s">
-        <v>135</v>
+        <v>80</v>
       </c>
       <c r="Y122" t="s">
         <v>0</v>
@@ -3106,7 +3100,7 @@
     </row>
     <row r="123" spans="21:25">
       <c r="U123" s="1" t="s">
-        <v>80</v>
+        <v>92</v>
       </c>
       <c r="Y123" t="s">
         <v>0</v>
@@ -3114,7 +3108,7 @@
     </row>
     <row r="124" spans="21:25">
       <c r="U124" s="1" t="s">
-        <v>81</v>
+        <v>138</v>
       </c>
       <c r="Y124" t="s">
         <v>0</v>
@@ -3122,7 +3116,7 @@
     </row>
     <row r="125" spans="21:25">
       <c r="U125" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="Y125" t="s">
         <v>0</v>
@@ -3130,7 +3124,7 @@
     </row>
     <row r="126" spans="21:25">
       <c r="U126" s="1" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
       <c r="Y126" t="s">
         <v>0</v>
@@ -3154,7 +3148,7 @@
     </row>
     <row r="129" spans="21:25">
       <c r="U129" s="1" t="s">
-        <v>85</v>
+        <v>100</v>
       </c>
       <c r="Y129" t="s">
         <v>0</v>
@@ -3162,7 +3156,7 @@
     </row>
     <row r="130" spans="21:25">
       <c r="U130" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="Y130" t="s">
         <v>0</v>
@@ -3170,7 +3164,7 @@
     </row>
     <row r="131" spans="21:25">
       <c r="U131" s="1" t="s">
-        <v>102</v>
+        <v>86</v>
       </c>
       <c r="Y131" t="s">
         <v>0</v>
@@ -3178,7 +3172,7 @@
     </row>
     <row r="132" spans="21:25">
       <c r="U132" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="Y132" t="s">
         <v>0</v>
@@ -3186,7 +3180,7 @@
     </row>
     <row r="133" spans="21:25">
       <c r="U133" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="Y133" t="s">
         <v>0</v>
@@ -3194,7 +3188,7 @@
     </row>
     <row r="134" spans="21:25">
       <c r="U134" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="Y134" t="s">
         <v>0</v>
@@ -3202,7 +3196,7 @@
     </row>
     <row r="135" spans="21:25">
       <c r="U135" s="1" t="s">
-        <v>89</v>
+        <v>133</v>
       </c>
       <c r="Y135" t="s">
         <v>0</v>
@@ -3210,7 +3204,7 @@
     </row>
     <row r="136" spans="21:25">
       <c r="U136" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="Y136" t="s">
         <v>0</v>
@@ -3218,24 +3212,20 @@
     </row>
     <row r="137" spans="21:25">
       <c r="U137" s="1" t="s">
-        <v>136</v>
+        <v>101</v>
       </c>
       <c r="Y137" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="138" spans="21:25">
-      <c r="U138" s="1" t="s">
-        <v>92</v>
-      </c>
+      <c r="U138" s="1"/>
       <c r="Y138" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="139" spans="21:25">
-      <c r="U139" s="1" t="s">
-        <v>103</v>
-      </c>
+      <c r="U139" s="1"/>
       <c r="Y139" t="s">
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
93.90 This is new score
</commit_message>
<xml_diff>
--- a/target debugger.xlsx
+++ b/target debugger.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\keegan\Downloads\A6Start\A6Start\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79DA0655-F249-4DBD-94A3-768B789517A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A62F241-AD3B-4D64-9453-C8BD2FE7E410}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{D1BDAA98-E73A-46CB-A5CF-2E613F0DCE3E}"/>
+    <workbookView xWindow="-38520" yWindow="-3255" windowWidth="38640" windowHeight="21240" xr2:uid="{D1BDAA98-E73A-46CB-A5CF-2E613F0DCE3E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,410 +36,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="579" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="536" uniqueCount="101">
   <si>
     <t>x</t>
   </si>
   <si>
-    <t>[x=0,y=0]</t>
-  </si>
-  <si>
-    <t>[x=0,y=2]</t>
-  </si>
-  <si>
-    <t>[x=2,y=0]</t>
-  </si>
-  <si>
-    <t>[x=2,y=2]</t>
-  </si>
-  <si>
-    <t>[x=5,y=13]</t>
-  </si>
-  <si>
-    <t>[x=5,y=1]</t>
-  </si>
-  <si>
-    <t>[x=1,y=3]</t>
-  </si>
-  <si>
-    <t>[x=5,y=9]</t>
-  </si>
-  <si>
-    <t>[x=7,y=13]</t>
-  </si>
-  <si>
-    <t>[x=7,y=1]</t>
-  </si>
-  <si>
-    <t>[x=4,y=0]</t>
-  </si>
-  <si>
-    <t>[x=4,y=2]</t>
-  </si>
-  <si>
-    <t>[x=3,y=9]</t>
-  </si>
-  <si>
-    <t>[x=3,y=1]</t>
-  </si>
-  <si>
-    <t>[x=6,y=0]</t>
-  </si>
-  <si>
-    <t>[x=6,y=2]</t>
-  </si>
-  <si>
-    <t>[x=0,y=9]</t>
-  </si>
-  <si>
-    <t>[x=3,y=13]</t>
-  </si>
-  <si>
-    <t>[x=8,y=0]</t>
-  </si>
-  <si>
-    <t>[x=8,y=2]</t>
-  </si>
-  <si>
-    <t>[x=10,y=2]</t>
-  </si>
-  <si>
-    <t>[x=12,y=0]</t>
-  </si>
-  <si>
-    <t>[x=11,y=13]</t>
-  </si>
-  <si>
-    <t>[x=9,y=1]</t>
-  </si>
-  <si>
-    <t>[x=9,y=13]</t>
-  </si>
-  <si>
-    <t>[x=9,y=9]</t>
-  </si>
-  <si>
-    <t>[x=13,y=13]</t>
-  </si>
-  <si>
-    <t>[x=10,y=7]</t>
-  </si>
-  <si>
-    <t>[x=11,y=7]</t>
-  </si>
-  <si>
-    <t>[x=4,y=14]</t>
-  </si>
-  <si>
-    <t>[x=6,y=10]</t>
-  </si>
-  <si>
-    <t>[x=12,y=5]</t>
-  </si>
-  <si>
-    <t>[x=11,y=5]</t>
-  </si>
-  <si>
-    <t>[x=4,y=10]</t>
-  </si>
-  <si>
-    <t>[x=6,y=14]</t>
-  </si>
-  <si>
-    <t>[x=9,y=5]</t>
-  </si>
-  <si>
-    <t>[x=2,y=14]</t>
-  </si>
-  <si>
-    <t>[x=2,y=10]</t>
-  </si>
-  <si>
-    <t>[x=3,y=5]</t>
-  </si>
-  <si>
-    <t>[x=1,y=11]</t>
-  </si>
-  <si>
-    <t>[x=0,y=5]</t>
-  </si>
-  <si>
-    <t>[x=3,y=7]</t>
-  </si>
-  <si>
-    <t>[x=10,y=14]</t>
-  </si>
-  <si>
-    <t>[x=4,y=7]</t>
-  </si>
-  <si>
-    <t>[x=8,y=14]</t>
-  </si>
-  <si>
-    <t>[x=5,y=5]</t>
-  </si>
-  <si>
-    <t>[x=7,y=7]</t>
-  </si>
-  <si>
-    <t>[x=10,y=10]</t>
-  </si>
-  <si>
-    <t>[x=7,y=11]</t>
-  </si>
-  <si>
-    <t>[x=5,y=11]</t>
-  </si>
-  <si>
-    <t>[x=3,y=11]</t>
-  </si>
-  <si>
-    <t>[x=1,y=7]</t>
-  </si>
-  <si>
-    <t>[x=1,y=5]</t>
-  </si>
-  <si>
-    <t>[x=13,y=11]</t>
-  </si>
-  <si>
-    <t>[x=11,y=11]</t>
-  </si>
-  <si>
-    <t>[x=6,y=12]</t>
-  </si>
-  <si>
-    <t>[x=8,y=8]</t>
-  </si>
-  <si>
-    <t>[x=12,y=6]</t>
-  </si>
-  <si>
-    <t>[x=11,y=8]</t>
-  </si>
-  <si>
-    <t>[x=4,y=12]</t>
-  </si>
-  <si>
-    <t>[x=12,y=8]</t>
-  </si>
-  <si>
-    <t>[x=10,y=6]</t>
-  </si>
-  <si>
-    <t>[x=8,y=4]</t>
-  </si>
-  <si>
-    <t>[x=12,y=3]</t>
-  </si>
-  <si>
-    <t>[x=10,y=4]</t>
-  </si>
-  <si>
-    <t>[x=2,y=12]</t>
-  </si>
-  <si>
-    <t>[x=12,y=4]</t>
-  </si>
-  <si>
-    <t>[x=9,y=3]</t>
-  </si>
-  <si>
-    <t>[x=11,y=3]</t>
-  </si>
-  <si>
-    <t>[x=1,y=1]</t>
-  </si>
-  <si>
-    <t>[x=2,y=8]</t>
-  </si>
-  <si>
-    <t>[x=3,y=6]</t>
-  </si>
-  <si>
-    <t>[x=4,y=4]</t>
-  </si>
-  <si>
-    <t>[x=7,y=3]</t>
-  </si>
-  <si>
-    <t>[x=1,y=13]</t>
-  </si>
-  <si>
-    <t>[x=2,y=6]</t>
-  </si>
-  <si>
-    <t>[x=5,y=3]</t>
-  </si>
-  <si>
-    <t>[x=1,y=9]</t>
-  </si>
-  <si>
-    <t>[x=0,y=4]</t>
-  </si>
-  <si>
-    <t>[x=2,y=4]</t>
-  </si>
-  <si>
-    <t>[x=3,y=3]</t>
-  </si>
-  <si>
-    <t>[x=4,y=8]</t>
-  </si>
-  <si>
-    <t>[x=6,y=6]</t>
-  </si>
-  <si>
-    <t>[x=12,y=12]</t>
-  </si>
-  <si>
-    <t>[x=5,y=8]</t>
-  </si>
-  <si>
-    <t>[x=14,y=12]</t>
-  </si>
-  <si>
-    <t>[x=0,y=3]</t>
-  </si>
-  <si>
-    <t>[x=4,y=6]</t>
-  </si>
-  <si>
-    <t>[x=8,y=12]</t>
-  </si>
-  <si>
-    <t>[x=10,y=12]</t>
-  </si>
-  <si>
-    <t>[x=1,y=4]</t>
-  </si>
-  <si>
-    <t>[x=1,y=2]</t>
-  </si>
-  <si>
-    <t>[x=1,y=10]</t>
-  </si>
-  <si>
-    <t>[x=1,y=12]</t>
-  </si>
-  <si>
-    <t>[x=1,y=8]</t>
-  </si>
-  <si>
-    <t>[x=5,y=2]</t>
-  </si>
-  <si>
-    <t>[x=7,y=2]</t>
-  </si>
-  <si>
-    <t>[x=3,y=2]</t>
-  </si>
-  <si>
-    <t>[x=5,y=14]</t>
-  </si>
-  <si>
-    <t>[x=13,y=12]</t>
-  </si>
-  <si>
-    <t>[x=11,y=12]</t>
-  </si>
-  <si>
     <t>P</t>
   </si>
   <si>
-    <t>[x=4,y=1]</t>
-  </si>
-  <si>
-    <t>[x=4,y=13]</t>
-  </si>
-  <si>
-    <t>[x=6,y=9]</t>
-  </si>
-  <si>
-    <t>[x=6,y=1]</t>
-  </si>
-  <si>
-    <t>[x=3,y=0]</t>
-  </si>
-  <si>
-    <t>[x=1,y=6]</t>
-  </si>
-  <si>
-    <t>[x=9,y=0]</t>
-  </si>
-  <si>
-    <t>[x=11,y=2]</t>
-  </si>
-  <si>
-    <t>[x=10,y=13]</t>
-  </si>
-  <si>
-    <t>[x=10,y=1]</t>
-  </si>
-  <si>
-    <t>[x=12,y=13]</t>
-  </si>
-  <si>
-    <t>[x=7,y=10]</t>
-  </si>
-  <si>
-    <t>[x=8,y=5]</t>
-  </si>
-  <si>
-    <t>[x=12,y=7]</t>
-  </si>
-  <si>
-    <t>[x=0,y=14]</t>
-  </si>
-  <si>
-    <t>[x=0,y=10]</t>
-  </si>
-  <si>
-    <t>[x=2,y=5]</t>
-  </si>
-  <si>
-    <t>[x=11,y=14]</t>
-  </si>
-  <si>
-    <t>[x=2,y=11]</t>
-  </si>
-  <si>
-    <t>[x=1,y=14]</t>
-  </si>
-  <si>
-    <t>[x=12,y=11]</t>
-  </si>
-  <si>
-    <t>[x=8,y=11]</t>
-  </si>
-  <si>
-    <t>[x=9,y=6]</t>
-  </si>
-  <si>
-    <t>[x=3,y=12]</t>
-  </si>
-  <si>
-    <t>[x=0,y=12]</t>
-  </si>
-  <si>
-    <t>[x=0,y=8]</t>
-  </si>
-  <si>
-    <t>[x=6,y=3]</t>
-  </si>
-  <si>
-    <t>[x=0,y=6]</t>
-  </si>
-  <si>
-    <t>[x=4,y=3]</t>
-  </si>
-  <si>
-    <t>[x=7,y=4]</t>
-  </si>
-  <si>
-    <t>[x=9,y=12]</t>
-  </si>
-  <si>
     <t>shots</t>
   </si>
   <si>
@@ -452,7 +56,289 @@
     <t>put hits here</t>
   </si>
   <si>
-    <t>[x=1,y=0]</t>
+    <t>java.awt.Point[x=1,y=12]</t>
+  </si>
+  <si>
+    <t>java.awt.Point[x=1,y=10]</t>
+  </si>
+  <si>
+    <t>java.awt.Point[x=2,y=7]</t>
+  </si>
+  <si>
+    <t>java.awt.Point[x=9,y=12]</t>
+  </si>
+  <si>
+    <t>java.awt.Point[x=9,y=14]</t>
+  </si>
+  <si>
+    <t>java.awt.Point[x=10,y=14]</t>
+  </si>
+  <si>
+    <t>java.awt.Point[x=11,y=14]</t>
+  </si>
+  <si>
+    <t>java.awt.Point[x=12,y=14]</t>
+  </si>
+  <si>
+    <t>java.awt.Point[x=8,y=14]</t>
+  </si>
+  <si>
+    <t>java.awt.Point[x=13,y=4]</t>
+  </si>
+  <si>
+    <t>java.awt.Point[x=13,y=2]</t>
+  </si>
+  <si>
+    <t>java.awt.Point[x=5,y=1]</t>
+  </si>
+  <si>
+    <t>java.awt.Point[x=5,y=9]</t>
+  </si>
+  <si>
+    <t>java.awt.Point[x=4,y=9]</t>
+  </si>
+  <si>
+    <t>java.awt.Point[x=5,y=0]</t>
+  </si>
+  <si>
+    <t>java.awt.Point[x=1,y=6]</t>
+  </si>
+  <si>
+    <t>java.awt.Point[x=7,y=2]</t>
+  </si>
+  <si>
+    <t>java.awt.Point[x=2,y=9]</t>
+  </si>
+  <si>
+    <t>java.awt.Point[x=11,y=13]</t>
+  </si>
+  <si>
+    <t>java.awt.Point[x=10,y=13]</t>
+  </si>
+  <si>
+    <t>java.awt.Point[x=9,y=9]</t>
+  </si>
+  <si>
+    <t>java.awt.Point[x=14,y=5]</t>
+  </si>
+  <si>
+    <t>java.awt.Point[x=10,y=5]</t>
+  </si>
+  <si>
+    <t>java.awt.Point[x=12,y=7]</t>
+  </si>
+  <si>
+    <t>java.awt.Point[x=0,y=7]</t>
+  </si>
+  <si>
+    <t>java.awt.Point[x=1,y=7]</t>
+  </si>
+  <si>
+    <t>java.awt.Point[x=0,y=11]</t>
+  </si>
+  <si>
+    <t>java.awt.Point[x=8,y=11]</t>
+  </si>
+  <si>
+    <t>java.awt.Point[x=4,y=12]</t>
+  </si>
+  <si>
+    <t>java.awt.Point[x=11,y=6]</t>
+  </si>
+  <si>
+    <t>java.awt.Point[x=9,y=4]</t>
+  </si>
+  <si>
+    <t>java.awt.Point[x=2,y=12]</t>
+  </si>
+  <si>
+    <t>java.awt.Point[x=8,y=3]</t>
+  </si>
+  <si>
+    <t>java.awt.Point[x=0,y=8]</t>
+  </si>
+  <si>
+    <t>java.awt.Point[x=0,y=6]</t>
+  </si>
+  <si>
+    <t>java.awt.Point[x=3,y=8]</t>
+  </si>
+  <si>
+    <t>java.awt.Point[x=1,y=0]</t>
+  </si>
+  <si>
+    <t>java.awt.Point[x=0,y=5]</t>
+  </si>
+  <si>
+    <t>pass</t>
+  </si>
+  <si>
+    <t>java.awt.Point[x=4,y=11]</t>
+  </si>
+  <si>
+    <t>java.awt.Point[x=8,y=7]</t>
+  </si>
+  <si>
+    <t>java.awt.Point[x=8,y=9]</t>
+  </si>
+  <si>
+    <t>java.awt.Point[x=7,y=9]</t>
+  </si>
+  <si>
+    <t>java.awt.Point[x=6,y=9]</t>
+  </si>
+  <si>
+    <t>java.awt.Point[x=11,y=10]</t>
+  </si>
+  <si>
+    <t>java.awt.Point[x=11,y=5]</t>
+  </si>
+  <si>
+    <t>java.awt.Point[x=3,y=12]</t>
+  </si>
+  <si>
+    <t>java.awt.Point[x=1,y=4]</t>
+  </si>
+  <si>
+    <t>java.awt.Point[x=4,y=1]</t>
+  </si>
+  <si>
+    <t>java.awt.Point[x=3,y=2]</t>
+  </si>
+  <si>
+    <t>java.awt.Point[x=3,y=0]</t>
+  </si>
+  <si>
+    <t>java.awt.Point[x=6,y=0]</t>
+  </si>
+  <si>
+    <t>java.awt.Point[x=0,y=9]</t>
+  </si>
+  <si>
+    <t>java.awt.Point[x=9,y=0]</t>
+  </si>
+  <si>
+    <t>java.awt.Point[x=11,y=2]</t>
+  </si>
+  <si>
+    <t>java.awt.Point[x=10,y=1]</t>
+  </si>
+  <si>
+    <t>java.awt.Point[x=2,y=5]</t>
+  </si>
+  <si>
+    <t>java.awt.Point[x=4,y=7]</t>
+  </si>
+  <si>
+    <t>java.awt.Point[x=2,y=11]</t>
+  </si>
+  <si>
+    <t>java.awt.Point[x=6,y=12]</t>
+  </si>
+  <si>
+    <t>java.awt.Point[x=12,y=6]</t>
+  </si>
+  <si>
+    <t>java.awt.Point[x=12,y=3]</t>
+  </si>
+  <si>
+    <t>java.awt.Point[x=10,y=4]</t>
+  </si>
+  <si>
+    <t>java.awt.Point[x=3,y=6]</t>
+  </si>
+  <si>
+    <t>java.awt.Point[x=1,y=2]</t>
+  </si>
+  <si>
+    <t>java.awt.Point[x=13,y=12]</t>
+  </si>
+  <si>
+    <t>java.awt.Point[x=5,y=8]</t>
+  </si>
+  <si>
+    <t>java.awt.Point[x=0,y=3]</t>
+  </si>
+  <si>
+    <t>worst case</t>
+  </si>
+  <si>
+    <t>java.awt.Point[x=13,y=7]</t>
+  </si>
+  <si>
+    <t>java.awt.Point[x=14,y=8]</t>
+  </si>
+  <si>
+    <t>java.awt.Point[x=12,y=1]</t>
+  </si>
+  <si>
+    <t>java.awt.Point[x=14,y=1]</t>
+  </si>
+  <si>
+    <t>java.awt.Point[x=6,y=5]</t>
+  </si>
+  <si>
+    <t>java.awt.Point[x=4,y=5]</t>
+  </si>
+  <si>
+    <t>java.awt.Point[x=13,y=8]</t>
+  </si>
+  <si>
+    <t>java.awt.Point[x=14,y=9]</t>
+  </si>
+  <si>
+    <t>java.awt.Point[x=0,y=1]</t>
+  </si>
+  <si>
+    <t>java.awt.Point[x=2,y=1]</t>
+  </si>
+  <si>
+    <t>java.awt.Point[x=12,y=11]</t>
+  </si>
+  <si>
+    <t>java.awt.Point[x=14,y=3]</t>
+  </si>
+  <si>
+    <t>java.awt.Point[x=7,y=6]</t>
+  </si>
+  <si>
+    <t>java.awt.Point[x=5,y=12]</t>
+  </si>
+  <si>
+    <t>java.awt.Point[x=0,y=13]</t>
+  </si>
+  <si>
+    <t>java.awt.Point[x=6,y=13]</t>
+  </si>
+  <si>
+    <t>java.awt.Point[x=2,y=13]</t>
+  </si>
+  <si>
+    <t>java.awt.Point[x=11,y=0]</t>
+  </si>
+  <si>
+    <t>java.awt.Point[x=9,y=8]</t>
+  </si>
+  <si>
+    <t>java.awt.Point[x=3,y=10]</t>
+  </si>
+  <si>
+    <t>java.awt.Point[x=5,y=4]</t>
+  </si>
+  <si>
+    <t>java.awt.Point[x=4,y=3]</t>
+  </si>
+  <si>
+    <t>java.awt.Point[x=2,y=3]</t>
+  </si>
+  <si>
+    <t>java.awt.Point[x=13,y=0]</t>
+  </si>
+  <si>
+    <t>java.awt.Point[x=14,y=13]</t>
+  </si>
+  <si>
+    <t>java.awt.Point[x=3,y=4]</t>
   </si>
 </sst>
 </file>
@@ -513,7 +399,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="10">
+  <dxfs count="3">
     <dxf>
       <font>
         <color rgb="FFFFC000"/>
@@ -521,16 +407,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -548,63 +424,6 @@
       <font>
         <color rgb="FFFF0000"/>
       </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00B0F0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00B0F0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00B0F0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <fill>
         <patternFill>
           <bgColor rgb="FFFF0000"/>
@@ -944,7 +763,7 @@
   <dimension ref="A1:AD389"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q9" sqref="Q9"/>
+      <selection activeCell="B20" sqref="B20:F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -956,27 +775,45 @@
   <sheetData>
     <row r="1" spans="1:30">
       <c r="R1" t="s">
-        <v>134</v>
+        <v>2</v>
       </c>
       <c r="S1">
         <f>COUNTA(U:U) -1</f>
-        <v>133</v>
+        <v>93</v>
       </c>
       <c r="U1" t="s">
-        <v>136</v>
+        <v>4</v>
       </c>
       <c r="AB1" t="s">
-        <v>137</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:30">
       <c r="R2" t="s">
-        <v>135</v>
+        <v>3</v>
       </c>
       <c r="S2" s="2">
         <f>S1/(15*15)</f>
-        <v>0.59111111111111114</v>
-      </c>
+        <v>0.41333333333333333</v>
+      </c>
+    </row>
+    <row r="3" spans="1:30">
+      <c r="R3" t="s">
+        <v>74</v>
+      </c>
+      <c r="S3">
+        <f>S1/(
+(15*15 /2)-(19)
+)</f>
+        <v>0.99465240641711228</v>
+      </c>
+    </row>
+    <row r="4" spans="1:30">
+      <c r="S4">
+        <f>(15*15 /2)-(19)</f>
+        <v>93.5</v>
+      </c>
+      <c r="AB4" s="1"/>
     </row>
     <row r="5" spans="1:30">
       <c r="B5">
@@ -1024,17 +861,16 @@
       <c r="P5">
         <v>14</v>
       </c>
-      <c r="U5" s="1" t="s">
+      <c r="Q5" t="s">
+        <v>44</v>
+      </c>
+      <c r="U5" s="1"/>
+      <c r="Y5" t="s">
+        <v>0</v>
+      </c>
+      <c r="AB5" s="1"/>
+      <c r="AD5" t="s">
         <v>1</v>
-      </c>
-      <c r="Y5" t="s">
-        <v>0</v>
-      </c>
-      <c r="AB5" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="AD5" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="6" spans="1:30">
@@ -1043,16 +879,16 @@
         <v>0</v>
       </c>
       <c r="B6" t="str">
-        <f>_xlfn.XLOOKUP("[x="&amp;B$5&amp;",y="&amp;$A6&amp;"]",$AB:$AB,$AD:$AD,_xlfn.XLOOKUP("[x="&amp;B$5&amp;",y="&amp;$A6&amp;"]",$U:$U,$Y:$Y,"o"))</f>
-        <v>x</v>
+        <f>_xlfn.XLOOKUP("java.awt.Point[x="&amp;B$5&amp;",y="&amp;$A6&amp;"]",$AB:$AB,$AD:$AD,_xlfn.XLOOKUP("java.awt.Point[x="&amp;B$5&amp;",y="&amp;$A6&amp;"]",$U:$U,$Y:$Y,"o"))</f>
+        <v>o</v>
       </c>
       <c r="C6" t="str">
-        <f t="shared" ref="C6:P20" si="0">_xlfn.XLOOKUP("[x="&amp;C$5&amp;",y="&amp;$A6&amp;"]",$AB:$AB,$AD:$AD,_xlfn.XLOOKUP("[x="&amp;C$5&amp;",y="&amp;$A6&amp;"]",$U:$U,$Y:$Y,"o"))</f>
+        <f t="shared" ref="C6:P6" si="0">_xlfn.XLOOKUP("java.awt.Point[x="&amp;C$5&amp;",y="&amp;$A6&amp;"]",$AB:$AB,$AD:$AD,_xlfn.XLOOKUP("java.awt.Point[x="&amp;C$5&amp;",y="&amp;$A6&amp;"]",$U:$U,$Y:$Y,"o"))</f>
         <v>x</v>
       </c>
       <c r="D6" t="str">
         <f t="shared" si="0"/>
-        <v>x</v>
+        <v>o</v>
       </c>
       <c r="E6" t="str">
         <f t="shared" si="0"/>
@@ -1060,11 +896,11 @@
       </c>
       <c r="F6" t="str">
         <f t="shared" si="0"/>
-        <v>x</v>
+        <v>o</v>
       </c>
       <c r="G6" t="str">
         <f t="shared" si="0"/>
-        <v>o</v>
+        <v>P</v>
       </c>
       <c r="H6" t="str">
         <f t="shared" si="0"/>
@@ -1076,7 +912,7 @@
       </c>
       <c r="J6" t="str">
         <f t="shared" si="0"/>
-        <v>x</v>
+        <v>o</v>
       </c>
       <c r="K6" t="str">
         <f t="shared" si="0"/>
@@ -1088,31 +924,43 @@
       </c>
       <c r="M6" t="str">
         <f t="shared" si="0"/>
-        <v>o</v>
+        <v>x</v>
       </c>
       <c r="N6" t="str">
         <f t="shared" si="0"/>
-        <v>x</v>
+        <v>o</v>
       </c>
       <c r="O6" t="str">
         <f t="shared" si="0"/>
-        <v>o</v>
+        <v>x</v>
       </c>
       <c r="P6" t="str">
         <f t="shared" si="0"/>
         <v>o</v>
       </c>
+      <c r="Q6" t="b">
+        <f>R6=S6</f>
+        <v>1</v>
+      </c>
+      <c r="R6">
+        <f>COUNTA(U:U)-1</f>
+        <v>93</v>
+      </c>
+      <c r="S6">
+        <f>COUNTA(_xlfn.UNIQUE(U5:U1048576))-1</f>
+        <v>93</v>
+      </c>
       <c r="U6" s="1" t="s">
-        <v>2</v>
+        <v>53</v>
       </c>
       <c r="Y6" t="s">
         <v>0</v>
       </c>
       <c r="AB6" s="1" t="s">
-        <v>91</v>
+        <v>30</v>
       </c>
       <c r="AD6" t="s">
-        <v>102</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:30">
@@ -1121,76 +969,88 @@
         <v>1</v>
       </c>
       <c r="B7" t="str">
-        <f t="shared" ref="B7:B20" si="1">_xlfn.XLOOKUP("[x="&amp;B$5&amp;",y="&amp;$A7&amp;"]",$AB:$AB,$AD:$AD,_xlfn.XLOOKUP("[x="&amp;B$5&amp;",y="&amp;$A7&amp;"]",$U:$U,$Y:$Y,"o"))</f>
-        <v>o</v>
+        <f t="shared" ref="B7:P20" si="1">_xlfn.XLOOKUP("java.awt.Point[x="&amp;B$5&amp;",y="&amp;$A7&amp;"]",$AB:$AB,$AD:$AD,_xlfn.XLOOKUP("java.awt.Point[x="&amp;B$5&amp;",y="&amp;$A7&amp;"]",$U:$U,$Y:$Y,"o"))</f>
+        <v>x</v>
       </c>
       <c r="C7" t="str">
-        <f t="shared" si="0"/>
-        <v>x</v>
+        <f t="shared" si="1"/>
+        <v>o</v>
       </c>
       <c r="D7" t="str">
-        <f t="shared" si="0"/>
-        <v>o</v>
+        <f t="shared" si="1"/>
+        <v>x</v>
       </c>
       <c r="E7" t="str">
-        <f t="shared" si="0"/>
-        <v>x</v>
+        <f t="shared" si="1"/>
+        <v>o</v>
       </c>
       <c r="F7" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>x</v>
       </c>
       <c r="G7" t="str">
-        <f t="shared" si="0"/>
-        <v>x</v>
+        <f t="shared" si="1"/>
+        <v>P</v>
       </c>
       <c r="H7" t="str">
-        <f t="shared" si="0"/>
-        <v>x</v>
+        <f t="shared" si="1"/>
+        <v>o</v>
       </c>
       <c r="I7" t="str">
-        <f t="shared" si="0"/>
-        <v>x</v>
+        <f t="shared" si="1"/>
+        <v>o</v>
       </c>
       <c r="J7" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>o</v>
       </c>
       <c r="K7" t="str">
-        <f t="shared" si="0"/>
-        <v>x</v>
+        <f t="shared" si="1"/>
+        <v>o</v>
       </c>
       <c r="L7" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>x</v>
       </c>
       <c r="M7" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>o</v>
       </c>
       <c r="N7" t="str">
-        <f t="shared" si="0"/>
-        <v>o</v>
+        <f t="shared" si="1"/>
+        <v>x</v>
       </c>
       <c r="O7" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>o</v>
       </c>
       <c r="P7" t="str">
-        <f t="shared" si="0"/>
-        <v>o</v>
+        <f t="shared" si="1"/>
+        <v>x</v>
+      </c>
+      <c r="Q7" t="b">
+        <f>R7=S7</f>
+        <v>1</v>
+      </c>
+      <c r="R7">
+        <f>COUNTA(AB:AB)-1</f>
+        <v>19</v>
+      </c>
+      <c r="S7">
+        <f>COUNTA(_xlfn.UNIQUE(AB5:AB249))-1</f>
+        <v>19</v>
       </c>
       <c r="U7" s="1" t="s">
-        <v>91</v>
+        <v>54</v>
       </c>
       <c r="Y7" t="s">
         <v>0</v>
       </c>
       <c r="AB7" s="1" t="s">
-        <v>53</v>
+        <v>39</v>
       </c>
       <c r="AD7" t="s">
-        <v>102</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:30">
@@ -1200,80 +1060,80 @@
       </c>
       <c r="B8" t="str">
         <f t="shared" si="1"/>
-        <v>x</v>
+        <v>o</v>
       </c>
       <c r="C8" t="str">
-        <f t="shared" si="0"/>
-        <v>P</v>
+        <f t="shared" si="1"/>
+        <v>x</v>
       </c>
       <c r="D8" t="str">
-        <f t="shared" si="0"/>
-        <v>x</v>
+        <f t="shared" si="1"/>
+        <v>o</v>
       </c>
       <c r="E8" t="str">
-        <f t="shared" si="0"/>
-        <v>P</v>
+        <f t="shared" si="1"/>
+        <v>x</v>
       </c>
       <c r="F8" t="str">
-        <f t="shared" si="0"/>
-        <v>P</v>
+        <f t="shared" si="1"/>
+        <v>o</v>
       </c>
       <c r="G8" t="str">
-        <f t="shared" si="0"/>
-        <v>P</v>
+        <f t="shared" si="1"/>
+        <v>o</v>
       </c>
       <c r="H8" t="str">
-        <f>_xlfn.XLOOKUP("[x="&amp;H$5&amp;",y="&amp;$A8&amp;"]",$AB:$AB,$AD:$AD,_xlfn.XLOOKUP("[x="&amp;H$5&amp;",y="&amp;$A8&amp;"]",$U:$U,$Y:$Y,"o"))</f>
-        <v>P</v>
+        <f t="shared" si="1"/>
+        <v>o</v>
       </c>
       <c r="I8" t="str">
-        <f t="shared" si="0"/>
-        <v>P</v>
+        <f t="shared" si="1"/>
+        <v>x</v>
       </c>
       <c r="J8" t="str">
-        <f t="shared" si="0"/>
-        <v>x</v>
+        <f t="shared" si="1"/>
+        <v>o</v>
       </c>
       <c r="K8" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>o</v>
       </c>
       <c r="L8" t="str">
-        <f t="shared" si="0"/>
-        <v>x</v>
+        <f t="shared" si="1"/>
+        <v>o</v>
       </c>
       <c r="M8" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>x</v>
       </c>
       <c r="N8" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>o</v>
       </c>
       <c r="O8" t="str">
-        <f t="shared" si="0"/>
-        <v>o</v>
+        <f t="shared" si="1"/>
+        <v>x</v>
       </c>
       <c r="P8" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>o</v>
       </c>
       <c r="U8" s="1" t="s">
-        <v>3</v>
+        <v>48</v>
       </c>
       <c r="Y8" t="s">
         <v>0</v>
       </c>
       <c r="AB8" s="1" t="s">
-        <v>92</v>
+        <v>58</v>
       </c>
       <c r="AD8" t="s">
-        <v>102</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:30">
       <c r="A9">
-        <f t="shared" ref="A9:A27" si="2">A8+1</f>
+        <f t="shared" ref="A9:A20" si="2">A8+1</f>
         <v>3</v>
       </c>
       <c r="B9" t="str">
@@ -1281,72 +1141,72 @@
         <v>x</v>
       </c>
       <c r="C9" t="str">
-        <f t="shared" si="0"/>
-        <v>P</v>
+        <f t="shared" si="1"/>
+        <v>o</v>
       </c>
       <c r="D9" t="str">
-        <f t="shared" si="0"/>
-        <v>o</v>
+        <f t="shared" si="1"/>
+        <v>x</v>
       </c>
       <c r="E9" t="str">
-        <f t="shared" si="0"/>
-        <v>x</v>
+        <f t="shared" si="1"/>
+        <v>o</v>
       </c>
       <c r="F9" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>x</v>
       </c>
       <c r="G9" t="str">
-        <f t="shared" si="0"/>
-        <v>x</v>
+        <f t="shared" si="1"/>
+        <v>o</v>
       </c>
       <c r="H9" t="str">
-        <f t="shared" si="0"/>
-        <v>x</v>
+        <f t="shared" si="1"/>
+        <v>o</v>
       </c>
       <c r="I9" t="str">
-        <f t="shared" si="0"/>
-        <v>x</v>
+        <f t="shared" si="1"/>
+        <v>o</v>
       </c>
       <c r="J9" t="str">
-        <f t="shared" si="0"/>
-        <v>o</v>
+        <f t="shared" si="1"/>
+        <v>x</v>
       </c>
       <c r="K9" t="str">
-        <f t="shared" si="0"/>
-        <v>x</v>
+        <f t="shared" si="1"/>
+        <v>o</v>
       </c>
       <c r="L9" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>o</v>
       </c>
       <c r="M9" t="str">
-        <f t="shared" si="0"/>
-        <v>x</v>
+        <f t="shared" si="1"/>
+        <v>o</v>
       </c>
       <c r="N9" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>x</v>
       </c>
       <c r="O9" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>o</v>
       </c>
       <c r="P9" t="str">
-        <f t="shared" si="0"/>
-        <v>o</v>
+        <f t="shared" si="1"/>
+        <v>x</v>
       </c>
       <c r="U9" s="1" t="s">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="Y9" t="s">
         <v>0</v>
       </c>
       <c r="AB9" s="1" t="s">
-        <v>95</v>
+        <v>52</v>
       </c>
       <c r="AD9" t="s">
-        <v>102</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:30">
@@ -1356,75 +1216,75 @@
       </c>
       <c r="B10" t="str">
         <f t="shared" si="1"/>
-        <v>x</v>
+        <v>o</v>
       </c>
       <c r="C10" t="str">
-        <f t="shared" si="0"/>
-        <v>P</v>
+        <f t="shared" si="1"/>
+        <v>x</v>
       </c>
       <c r="D10" t="str">
-        <f t="shared" si="0"/>
-        <v>x</v>
+        <f t="shared" si="1"/>
+        <v>o</v>
       </c>
       <c r="E10" t="str">
-        <f t="shared" si="0"/>
-        <v>o</v>
+        <f t="shared" si="1"/>
+        <v>x</v>
       </c>
       <c r="F10" t="str">
-        <f t="shared" si="0"/>
-        <v>x</v>
+        <f>_xlfn.XLOOKUP("java.awt.Point[x="&amp;F$5&amp;",y="&amp;$A10&amp;"]",$AB:$AB,$AD:$AD,_xlfn.XLOOKUP("java.awt.Point[x="&amp;F$5&amp;",y="&amp;$A10&amp;"]",$U:$U,$Y:$Y,"o"))</f>
+        <v>o</v>
       </c>
       <c r="G10" t="str">
-        <f t="shared" si="0"/>
-        <v>o</v>
+        <f t="shared" si="1"/>
+        <v>x</v>
       </c>
       <c r="H10" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>o</v>
       </c>
       <c r="I10" t="str">
-        <f t="shared" si="0"/>
-        <v>x</v>
+        <f t="shared" si="1"/>
+        <v>o</v>
       </c>
       <c r="J10" t="str">
-        <f t="shared" si="0"/>
-        <v>x</v>
+        <f t="shared" si="1"/>
+        <v>o</v>
       </c>
       <c r="K10" t="str">
-        <f t="shared" si="0"/>
-        <v>o</v>
+        <f t="shared" si="1"/>
+        <v>x</v>
       </c>
       <c r="L10" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>x</v>
       </c>
       <c r="M10" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>o</v>
       </c>
       <c r="N10" t="str">
-        <f t="shared" si="0"/>
-        <v>P</v>
+        <f t="shared" si="1"/>
+        <v>o</v>
       </c>
       <c r="O10" t="str">
-        <f t="shared" si="0"/>
-        <v>o</v>
+        <f t="shared" si="1"/>
+        <v>x</v>
       </c>
       <c r="P10" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>o</v>
       </c>
       <c r="U10" s="1" t="s">
-        <v>103</v>
+        <v>49</v>
       </c>
       <c r="Y10" t="s">
         <v>0</v>
       </c>
       <c r="AB10" s="1" t="s">
-        <v>78</v>
+        <v>34</v>
       </c>
       <c r="AD10" t="s">
-        <v>102</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:30">
@@ -1437,72 +1297,72 @@
         <v>x</v>
       </c>
       <c r="C11" t="str">
-        <f t="shared" si="0"/>
-        <v>P</v>
+        <f t="shared" si="1"/>
+        <v>o</v>
       </c>
       <c r="D11" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>x</v>
       </c>
       <c r="E11" t="str">
-        <f t="shared" si="0"/>
-        <v>x</v>
+        <f t="shared" si="1"/>
+        <v>o</v>
       </c>
       <c r="F11" t="str">
-        <f t="shared" si="0"/>
-        <v>o</v>
+        <f t="shared" si="1"/>
+        <v>x</v>
       </c>
       <c r="G11" t="str">
-        <f t="shared" si="0"/>
-        <v>x</v>
+        <f t="shared" si="1"/>
+        <v>o</v>
       </c>
       <c r="H11" t="str">
-        <f t="shared" si="0"/>
-        <v>o</v>
+        <f t="shared" si="1"/>
+        <v>x</v>
       </c>
       <c r="I11" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>o</v>
       </c>
       <c r="J11" t="str">
-        <f t="shared" si="0"/>
-        <v>x</v>
+        <f t="shared" si="1"/>
+        <v>o</v>
       </c>
       <c r="K11" t="str">
-        <f t="shared" si="0"/>
-        <v>x</v>
+        <f t="shared" si="1"/>
+        <v>o</v>
       </c>
       <c r="L11" t="str">
-        <f t="shared" si="0"/>
-        <v>o</v>
+        <f t="shared" si="1"/>
+        <v>x</v>
       </c>
       <c r="M11" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>x</v>
       </c>
       <c r="N11" t="str">
-        <f t="shared" si="0"/>
-        <v>P</v>
+        <f t="shared" si="1"/>
+        <v>o</v>
       </c>
       <c r="O11" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>o</v>
       </c>
       <c r="P11" t="str">
-        <f t="shared" si="0"/>
-        <v>o</v>
+        <f t="shared" si="1"/>
+        <v>x</v>
       </c>
       <c r="U11" s="1" t="s">
-        <v>5</v>
+        <v>56</v>
       </c>
       <c r="Y11" t="s">
         <v>0</v>
       </c>
       <c r="AB11" s="1" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="AD11" t="s">
-        <v>102</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:30">
@@ -1515,72 +1375,72 @@
         <v>x</v>
       </c>
       <c r="C12" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>x</v>
       </c>
       <c r="D12" t="str">
-        <f t="shared" si="0"/>
-        <v>x</v>
+        <f t="shared" si="1"/>
+        <v>o</v>
       </c>
       <c r="E12" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>x</v>
       </c>
       <c r="F12" t="str">
-        <f t="shared" si="0"/>
-        <v>x</v>
+        <f t="shared" si="1"/>
+        <v>o</v>
       </c>
       <c r="G12" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>o</v>
       </c>
       <c r="H12" t="str">
-        <f t="shared" si="0"/>
-        <v>x</v>
+        <f t="shared" si="1"/>
+        <v>o</v>
       </c>
       <c r="I12" t="str">
-        <f t="shared" si="0"/>
-        <v>o</v>
+        <f t="shared" si="1"/>
+        <v>x</v>
       </c>
       <c r="J12" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>o</v>
       </c>
       <c r="K12" t="str">
-        <f t="shared" si="0"/>
-        <v>x</v>
+        <f t="shared" si="1"/>
+        <v>o</v>
       </c>
       <c r="L12" t="str">
-        <f t="shared" si="0"/>
-        <v>x</v>
+        <f t="shared" si="1"/>
+        <v>o</v>
       </c>
       <c r="M12" t="str">
-        <f t="shared" si="0"/>
-        <v>o</v>
+        <f t="shared" si="1"/>
+        <v>x</v>
       </c>
       <c r="N12" t="str">
-        <f t="shared" si="0"/>
-        <v>P</v>
+        <f t="shared" si="1"/>
+        <v>x</v>
       </c>
       <c r="O12" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>o</v>
       </c>
       <c r="P12" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>o</v>
       </c>
       <c r="U12" s="1" t="s">
-        <v>6</v>
+        <v>55</v>
       </c>
       <c r="Y12" t="s">
         <v>0</v>
       </c>
       <c r="AB12" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="AD12" t="s">
-        <v>102</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:30">
@@ -1590,75 +1450,75 @@
       </c>
       <c r="B13" t="str">
         <f t="shared" si="1"/>
-        <v>o</v>
+        <v>P</v>
       </c>
       <c r="C13" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>x</v>
       </c>
       <c r="D13" t="str">
-        <f t="shared" si="0"/>
-        <v>o</v>
+        <f t="shared" si="1"/>
+        <v>x</v>
       </c>
       <c r="E13" t="str">
-        <f t="shared" si="0"/>
-        <v>x</v>
+        <f t="shared" si="1"/>
+        <v>o</v>
       </c>
       <c r="F13" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>x</v>
       </c>
       <c r="G13" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>o</v>
       </c>
       <c r="H13" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>o</v>
       </c>
       <c r="I13" t="str">
-        <f t="shared" si="0"/>
-        <v>x</v>
+        <f t="shared" si="1"/>
+        <v>o</v>
       </c>
       <c r="J13" t="str">
-        <f t="shared" si="0"/>
-        <v>o</v>
+        <f t="shared" si="1"/>
+        <v>x</v>
       </c>
       <c r="K13" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>o</v>
       </c>
       <c r="L13" t="str">
-        <f t="shared" si="0"/>
-        <v>x</v>
+        <f t="shared" si="1"/>
+        <v>o</v>
       </c>
       <c r="M13" t="str">
-        <f t="shared" si="0"/>
-        <v>x</v>
+        <f t="shared" si="1"/>
+        <v>o</v>
       </c>
       <c r="N13" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>x</v>
       </c>
       <c r="O13" t="str">
-        <f t="shared" si="0"/>
-        <v>o</v>
+        <f t="shared" si="1"/>
+        <v>x</v>
       </c>
       <c r="P13" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>o</v>
       </c>
       <c r="U13" s="1" t="s">
-        <v>104</v>
+        <v>18</v>
       </c>
       <c r="Y13" t="s">
         <v>0</v>
       </c>
       <c r="AB13" s="1" t="s">
-        <v>94</v>
+        <v>19</v>
       </c>
       <c r="AD13" t="s">
-        <v>102</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:30">
@@ -1668,75 +1528,75 @@
       </c>
       <c r="B14" t="str">
         <f t="shared" si="1"/>
-        <v>x</v>
+        <v>P</v>
       </c>
       <c r="C14" t="str">
-        <f t="shared" si="0"/>
-        <v>P</v>
+        <f t="shared" si="1"/>
+        <v>o</v>
       </c>
       <c r="D14" t="str">
-        <f t="shared" si="0"/>
-        <v>x</v>
+        <f t="shared" si="1"/>
+        <v>o</v>
       </c>
       <c r="E14" t="str">
-        <f t="shared" si="0"/>
-        <v>o</v>
+        <f t="shared" si="1"/>
+        <v>x</v>
       </c>
       <c r="F14" t="str">
-        <f t="shared" si="0"/>
-        <v>x</v>
+        <f t="shared" si="1"/>
+        <v>o</v>
       </c>
       <c r="G14" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>x</v>
       </c>
       <c r="H14" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>o</v>
       </c>
       <c r="I14" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>o</v>
       </c>
       <c r="J14" t="str">
-        <f t="shared" si="0"/>
-        <v>x</v>
+        <f t="shared" si="1"/>
+        <v>o</v>
       </c>
       <c r="K14" t="str">
-        <f t="shared" si="0"/>
-        <v>o</v>
+        <f t="shared" si="1"/>
+        <v>x</v>
       </c>
       <c r="L14" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>o</v>
       </c>
       <c r="M14" t="str">
-        <f t="shared" si="0"/>
-        <v>x</v>
+        <f t="shared" si="1"/>
+        <v>o</v>
       </c>
       <c r="N14" t="str">
-        <f t="shared" si="0"/>
-        <v>x</v>
+        <f t="shared" si="1"/>
+        <v>o</v>
       </c>
       <c r="O14" t="str">
-        <f t="shared" si="0"/>
-        <v>o</v>
+        <f t="shared" si="1"/>
+        <v>x</v>
       </c>
       <c r="P14" t="str">
-        <f t="shared" si="0"/>
-        <v>o</v>
+        <f t="shared" si="1"/>
+        <v>x</v>
       </c>
       <c r="U14" s="1" t="s">
-        <v>105</v>
+        <v>45</v>
       </c>
       <c r="Y14" t="s">
         <v>0</v>
       </c>
       <c r="AB14" s="1" t="s">
-        <v>75</v>
+        <v>18</v>
       </c>
       <c r="AD14" t="s">
-        <v>102</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:30">
@@ -1746,75 +1606,75 @@
       </c>
       <c r="B15" t="str">
         <f t="shared" si="1"/>
-        <v>x</v>
+        <v>P</v>
       </c>
       <c r="C15" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
+        <v>o</v>
+      </c>
+      <c r="D15" t="str">
+        <f t="shared" si="1"/>
+        <v>x</v>
+      </c>
+      <c r="E15" t="str">
+        <f t="shared" si="1"/>
+        <v>o</v>
+      </c>
+      <c r="F15" t="str">
+        <f t="shared" si="1"/>
         <v>P</v>
       </c>
-      <c r="D15" t="str">
-        <f t="shared" si="0"/>
-        <v>o</v>
-      </c>
-      <c r="E15" t="str">
-        <f t="shared" si="0"/>
-        <v>x</v>
-      </c>
-      <c r="F15" t="str">
-        <f t="shared" si="0"/>
-        <v>o</v>
-      </c>
       <c r="G15" t="str">
-        <f t="shared" si="0"/>
-        <v>x</v>
+        <f t="shared" si="1"/>
+        <v>P</v>
       </c>
       <c r="H15" t="str">
-        <f t="shared" si="0"/>
-        <v>x</v>
+        <f t="shared" si="1"/>
+        <v>P</v>
       </c>
       <c r="I15" t="str">
-        <f t="shared" si="0"/>
-        <v>o</v>
+        <f t="shared" si="1"/>
+        <v>P</v>
       </c>
       <c r="J15" t="str">
-        <f t="shared" si="0"/>
-        <v>o</v>
+        <f t="shared" si="1"/>
+        <v>P</v>
       </c>
       <c r="K15" t="str">
-        <f t="shared" si="0"/>
-        <v>x</v>
+        <f t="shared" si="1"/>
+        <v>P</v>
       </c>
       <c r="L15" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>o</v>
       </c>
       <c r="M15" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>o</v>
       </c>
       <c r="N15" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>o</v>
       </c>
       <c r="O15" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>o</v>
       </c>
       <c r="P15" t="str">
-        <f t="shared" si="0"/>
-        <v>o</v>
+        <f t="shared" si="1"/>
+        <v>x</v>
       </c>
       <c r="U15" s="1" t="s">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="Y15" t="s">
         <v>0</v>
       </c>
       <c r="AB15" s="1" t="s">
-        <v>12</v>
+        <v>49</v>
       </c>
       <c r="AD15" t="s">
-        <v>102</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:30">
@@ -1824,75 +1684,75 @@
       </c>
       <c r="B16" t="str">
         <f t="shared" si="1"/>
-        <v>x</v>
+        <v>o</v>
       </c>
       <c r="C16" t="str">
-        <f t="shared" si="0"/>
-        <v>P</v>
+        <f t="shared" si="1"/>
+        <v>x</v>
       </c>
       <c r="D16" t="str">
-        <f t="shared" si="0"/>
-        <v>x</v>
+        <f t="shared" si="1"/>
+        <v>o</v>
       </c>
       <c r="E16" t="str">
-        <f t="shared" si="0"/>
-        <v>o</v>
+        <f t="shared" si="1"/>
+        <v>x</v>
       </c>
       <c r="F16" t="str">
-        <f t="shared" si="0"/>
-        <v>x</v>
+        <f t="shared" si="1"/>
+        <v>o</v>
       </c>
       <c r="G16" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>o</v>
       </c>
       <c r="H16" t="str">
-        <f t="shared" si="0"/>
-        <v>x</v>
+        <f t="shared" si="1"/>
+        <v>o</v>
       </c>
       <c r="I16" t="str">
-        <f t="shared" si="0"/>
-        <v>x</v>
+        <f t="shared" si="1"/>
+        <v>o</v>
       </c>
       <c r="J16" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>o</v>
       </c>
       <c r="K16" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>o</v>
       </c>
       <c r="L16" t="str">
-        <f t="shared" si="0"/>
-        <v>x</v>
+        <f t="shared" si="1"/>
+        <v>o</v>
       </c>
       <c r="M16" t="str">
-        <f t="shared" si="0"/>
-        <v>o</v>
+        <f t="shared" si="1"/>
+        <v>x</v>
       </c>
       <c r="N16" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>o</v>
       </c>
       <c r="O16" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>o</v>
       </c>
       <c r="P16" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>o</v>
       </c>
       <c r="U16" s="1" t="s">
-        <v>106</v>
+        <v>90</v>
       </c>
       <c r="Y16" t="s">
         <v>0</v>
       </c>
       <c r="AB16" s="1" t="s">
-        <v>96</v>
+        <v>48</v>
       </c>
       <c r="AD16" t="s">
-        <v>102</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:30">
@@ -1902,75 +1762,75 @@
       </c>
       <c r="B17" t="str">
         <f t="shared" si="1"/>
-        <v>o</v>
+        <v>x</v>
       </c>
       <c r="C17" t="str">
-        <f t="shared" si="0"/>
-        <v>P</v>
+        <f t="shared" si="1"/>
+        <v>o</v>
       </c>
       <c r="D17" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>x</v>
       </c>
       <c r="E17" t="str">
-        <f t="shared" si="0"/>
-        <v>x</v>
+        <f t="shared" si="1"/>
+        <v>o</v>
       </c>
       <c r="F17" t="str">
-        <f t="shared" si="0"/>
-        <v>o</v>
+        <f t="shared" si="1"/>
+        <v>x</v>
       </c>
       <c r="G17" t="str">
-        <f t="shared" si="0"/>
-        <v>x</v>
+        <f t="shared" si="1"/>
+        <v>o</v>
       </c>
       <c r="H17" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>o</v>
       </c>
       <c r="I17" t="str">
-        <f t="shared" si="0"/>
-        <v>x</v>
+        <f t="shared" si="1"/>
+        <v>o</v>
       </c>
       <c r="J17" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>x</v>
       </c>
       <c r="K17" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>o</v>
       </c>
       <c r="L17" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>o</v>
       </c>
       <c r="M17" t="str">
-        <f t="shared" si="0"/>
-        <v>x</v>
+        <f t="shared" si="1"/>
+        <v>o</v>
       </c>
       <c r="N17" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>x</v>
       </c>
       <c r="O17" t="str">
-        <f t="shared" si="0"/>
-        <v>x</v>
+        <f t="shared" si="1"/>
+        <v>o</v>
       </c>
       <c r="P17" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>o</v>
       </c>
       <c r="U17" s="1" t="s">
-        <v>98</v>
+        <v>83</v>
       </c>
       <c r="Y17" t="s">
         <v>0</v>
       </c>
       <c r="AB17" s="1" t="s">
-        <v>16</v>
+        <v>47</v>
       </c>
       <c r="AD17" t="s">
-        <v>102</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:30">
@@ -1980,75 +1840,75 @@
       </c>
       <c r="B18" t="str">
         <f t="shared" si="1"/>
-        <v>x</v>
+        <v>o</v>
       </c>
       <c r="C18" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
+        <v>x</v>
+      </c>
+      <c r="D18" t="str">
+        <f t="shared" si="1"/>
         <v>P</v>
       </c>
-      <c r="D18" t="str">
-        <f t="shared" si="0"/>
-        <v>x</v>
-      </c>
       <c r="E18" t="str">
-        <f t="shared" si="0"/>
-        <v>x</v>
+        <f t="shared" si="1"/>
+        <v>P</v>
       </c>
       <c r="F18" t="str">
-        <f t="shared" si="0"/>
-        <v>x</v>
+        <f t="shared" si="1"/>
+        <v>P</v>
       </c>
       <c r="G18" t="str">
-        <f t="shared" si="0"/>
-        <v>o</v>
+        <f t="shared" si="1"/>
+        <v>P</v>
       </c>
       <c r="H18" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>x</v>
       </c>
       <c r="I18" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>o</v>
       </c>
       <c r="J18" t="str">
-        <f t="shared" si="0"/>
-        <v>x</v>
+        <f t="shared" si="1"/>
+        <v>o</v>
       </c>
       <c r="K18" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>x</v>
       </c>
       <c r="L18" t="str">
-        <f t="shared" si="0"/>
-        <v>P</v>
+        <f t="shared" si="1"/>
+        <v>o</v>
       </c>
       <c r="M18" t="str">
-        <f t="shared" si="0"/>
-        <v>P</v>
+        <f t="shared" si="1"/>
+        <v>o</v>
       </c>
       <c r="N18" t="str">
-        <f t="shared" si="0"/>
-        <v>P</v>
+        <f t="shared" si="1"/>
+        <v>o</v>
       </c>
       <c r="O18" t="str">
-        <f t="shared" si="0"/>
-        <v>P</v>
+        <f t="shared" si="1"/>
+        <v>x</v>
       </c>
       <c r="P18" t="str">
-        <f t="shared" si="0"/>
-        <v>x</v>
+        <f t="shared" si="1"/>
+        <v>o</v>
       </c>
       <c r="U18" s="1" t="s">
-        <v>107</v>
+        <v>84</v>
       </c>
       <c r="Y18" t="s">
         <v>0</v>
       </c>
       <c r="AB18" s="1" t="s">
-        <v>97</v>
+        <v>26</v>
       </c>
       <c r="AD18" t="s">
-        <v>102</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:30">
@@ -2058,75 +1918,75 @@
       </c>
       <c r="B19" t="str">
         <f t="shared" si="1"/>
-        <v>o</v>
+        <v>x</v>
       </c>
       <c r="C19" t="str">
-        <f t="shared" si="0"/>
-        <v>P</v>
+        <f t="shared" si="1"/>
+        <v>o</v>
       </c>
       <c r="D19" t="str">
-        <f t="shared" si="0"/>
-        <v>o</v>
+        <f t="shared" si="1"/>
+        <v>x</v>
       </c>
       <c r="E19" t="str">
-        <f t="shared" si="0"/>
-        <v>x</v>
+        <f t="shared" si="1"/>
+        <v>o</v>
       </c>
       <c r="F19" t="str">
-        <f t="shared" si="0"/>
-        <v>x</v>
+        <f t="shared" si="1"/>
+        <v>o</v>
       </c>
       <c r="G19" t="str">
-        <f t="shared" si="0"/>
-        <v>x</v>
+        <f t="shared" si="1"/>
+        <v>o</v>
       </c>
       <c r="H19" t="str">
-        <f t="shared" si="0"/>
-        <v>o</v>
+        <f t="shared" si="1"/>
+        <v>x</v>
       </c>
       <c r="I19" t="str">
-        <f t="shared" si="0"/>
-        <v>x</v>
+        <f t="shared" si="1"/>
+        <v>o</v>
       </c>
       <c r="J19" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>o</v>
       </c>
       <c r="K19" t="str">
-        <f t="shared" si="0"/>
-        <v>x</v>
+        <f t="shared" si="1"/>
+        <v>o</v>
       </c>
       <c r="L19" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>x</v>
       </c>
       <c r="M19" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>x</v>
       </c>
       <c r="N19" t="str">
-        <f t="shared" si="0"/>
-        <v>x</v>
+        <f t="shared" si="1"/>
+        <v>o</v>
       </c>
       <c r="O19" t="str">
-        <f t="shared" si="0"/>
-        <v>x</v>
+        <f t="shared" si="1"/>
+        <v>o</v>
       </c>
       <c r="P19" t="str">
-        <f t="shared" si="0"/>
-        <v>o</v>
+        <f t="shared" si="1"/>
+        <v>x</v>
       </c>
       <c r="U19" s="1" t="s">
-        <v>9</v>
+        <v>31</v>
       </c>
       <c r="Y19" t="s">
         <v>0</v>
       </c>
       <c r="AB19" s="1" t="s">
-        <v>98</v>
+        <v>20</v>
       </c>
       <c r="AD19" t="s">
-        <v>102</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:30">
@@ -2136,1084 +1996,1085 @@
       </c>
       <c r="B20" t="str">
         <f t="shared" si="1"/>
-        <v>x</v>
+        <v>o</v>
       </c>
       <c r="C20" t="str">
-        <f t="shared" si="0"/>
-        <v>x</v>
+        <f t="shared" si="1"/>
+        <v>o</v>
       </c>
       <c r="D20" t="str">
-        <f t="shared" si="0"/>
-        <v>x</v>
+        <f t="shared" si="1"/>
+        <v>o</v>
       </c>
       <c r="E20" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>o</v>
       </c>
       <c r="F20" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
+        <v>o</v>
+      </c>
+      <c r="G20" t="str">
+        <f t="shared" si="1"/>
+        <v>o</v>
+      </c>
+      <c r="H20" t="str">
+        <f t="shared" si="1"/>
+        <v>o</v>
+      </c>
+      <c r="I20" t="str">
+        <f t="shared" si="1"/>
+        <v>o</v>
+      </c>
+      <c r="J20" t="str">
+        <f t="shared" si="1"/>
         <v>P</v>
       </c>
-      <c r="G20" t="str">
-        <f t="shared" si="0"/>
+      <c r="K20" t="str">
+        <f t="shared" si="1"/>
         <v>P</v>
       </c>
-      <c r="H20" t="str">
-        <f t="shared" si="0"/>
-        <v>x</v>
-      </c>
-      <c r="I20" t="str">
-        <f t="shared" si="0"/>
-        <v>o</v>
-      </c>
-      <c r="J20" t="str">
-        <f t="shared" si="0"/>
-        <v>x</v>
-      </c>
-      <c r="K20" t="str">
-        <f t="shared" si="0"/>
-        <v>o</v>
-      </c>
       <c r="L20" t="str">
-        <f t="shared" si="0"/>
-        <v>x</v>
+        <f t="shared" si="1"/>
+        <v>P</v>
       </c>
       <c r="M20" t="str">
-        <f t="shared" si="0"/>
-        <v>x</v>
+        <f t="shared" si="1"/>
+        <v>P</v>
       </c>
       <c r="N20" t="str">
-        <f t="shared" si="0"/>
-        <v>o</v>
+        <f t="shared" si="1"/>
+        <v>x</v>
       </c>
       <c r="O20" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>o</v>
       </c>
       <c r="P20" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>o</v>
       </c>
       <c r="U20" s="1" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="Y20" t="s">
         <v>0</v>
       </c>
       <c r="AB20" s="1" t="s">
-        <v>30</v>
+        <v>17</v>
       </c>
       <c r="AD20" t="s">
-        <v>102</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:30">
       <c r="U21" s="1" t="s">
-        <v>10</v>
+        <v>89</v>
       </c>
       <c r="Y21" t="s">
         <v>0</v>
       </c>
       <c r="AB21" s="1" t="s">
-        <v>99</v>
+        <v>12</v>
       </c>
       <c r="AD21" t="s">
-        <v>102</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:30">
       <c r="U22" s="1" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="Y22" t="s">
         <v>0</v>
       </c>
       <c r="AB22" s="1" t="s">
-        <v>58</v>
+        <v>11</v>
       </c>
       <c r="AD22" t="s">
-        <v>102</v>
+        <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:30">
       <c r="U23" s="1" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="Y23" t="s">
         <v>0</v>
       </c>
       <c r="AB23" s="1" t="s">
-        <v>32</v>
+        <v>10</v>
       </c>
       <c r="AD23" t="s">
-        <v>102</v>
+        <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:30">
       <c r="U24" s="1" t="s">
-        <v>12</v>
+        <v>57</v>
       </c>
       <c r="Y24" t="s">
         <v>0</v>
       </c>
       <c r="AB24" s="1" t="s">
-        <v>67</v>
+        <v>14</v>
       </c>
       <c r="AD24" t="s">
-        <v>102</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:30">
       <c r="U25" s="1" t="s">
-        <v>96</v>
+        <v>32</v>
       </c>
       <c r="Y25" t="s">
         <v>0</v>
       </c>
-      <c r="AB25" s="1" t="s">
-        <v>84</v>
-      </c>
+      <c r="AB25" s="1"/>
       <c r="AD25" t="s">
-        <v>102</v>
+        <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:30">
       <c r="U26" s="1" t="s">
-        <v>13</v>
+        <v>64</v>
       </c>
       <c r="Y26" t="s">
         <v>0</v>
       </c>
-      <c r="AB26" s="1" t="s">
-        <v>100</v>
-      </c>
+      <c r="AB26" s="1"/>
       <c r="AD26" t="s">
-        <v>102</v>
+        <v>1</v>
       </c>
     </row>
     <row r="27" spans="1:30">
       <c r="U27" s="1" t="s">
-        <v>108</v>
+        <v>22</v>
       </c>
       <c r="Y27" t="s">
         <v>0</v>
       </c>
-      <c r="AB27" s="1" t="s">
-        <v>101</v>
-      </c>
+      <c r="AB27" s="1"/>
       <c r="AD27" t="s">
-        <v>102</v>
+        <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:30">
       <c r="U28" s="1" t="s">
-        <v>14</v>
+        <v>58</v>
       </c>
       <c r="Y28" t="s">
         <v>0</v>
       </c>
-      <c r="AB28" s="1" t="s">
-        <v>90</v>
-      </c>
+      <c r="AB28" s="1"/>
       <c r="AD28" t="s">
-        <v>102</v>
+        <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:30">
       <c r="U29" s="1" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="Y29" t="s">
         <v>0</v>
       </c>
+      <c r="AB29" s="1"/>
       <c r="AD29" t="s">
-        <v>102</v>
+        <v>1</v>
       </c>
     </row>
     <row r="30" spans="1:30">
       <c r="U30" s="1" t="s">
-        <v>15</v>
+        <v>59</v>
       </c>
       <c r="Y30" t="s">
         <v>0</v>
       </c>
+      <c r="AB30" s="1"/>
       <c r="AD30" t="s">
-        <v>102</v>
+        <v>1</v>
       </c>
     </row>
     <row r="31" spans="1:30">
       <c r="U31" s="1" t="s">
-        <v>97</v>
+        <v>60</v>
       </c>
       <c r="Y31" t="s">
         <v>0</v>
       </c>
+      <c r="AB31" s="1"/>
       <c r="AD31" t="s">
-        <v>102</v>
+        <v>1</v>
       </c>
     </row>
     <row r="32" spans="1:30">
       <c r="U32" s="1" t="s">
-        <v>18</v>
+        <v>92</v>
       </c>
       <c r="Y32" t="s">
         <v>0</v>
       </c>
+      <c r="AB32" s="1"/>
       <c r="AD32" t="s">
-        <v>102</v>
+        <v>1</v>
       </c>
     </row>
     <row r="33" spans="21:30">
       <c r="U33" s="1" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="Y33" t="s">
         <v>0</v>
       </c>
+      <c r="AB33" s="1"/>
       <c r="AD33" t="s">
-        <v>102</v>
+        <v>1</v>
       </c>
     </row>
     <row r="34" spans="21:30">
       <c r="U34" s="1" t="s">
-        <v>20</v>
+        <v>98</v>
       </c>
       <c r="Y34" t="s">
         <v>0</v>
       </c>
+      <c r="AB34" s="1"/>
       <c r="AD34" t="s">
-        <v>102</v>
+        <v>1</v>
       </c>
     </row>
     <row r="35" spans="21:30">
       <c r="U35" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="Y35" t="s">
         <v>0</v>
       </c>
+      <c r="AB35" s="1"/>
       <c r="AD35" t="s">
-        <v>102</v>
+        <v>1</v>
       </c>
     </row>
     <row r="36" spans="21:30">
       <c r="U36" s="1" t="s">
-        <v>109</v>
+        <v>7</v>
       </c>
       <c r="Y36" t="s">
         <v>0</v>
       </c>
+      <c r="AB36" s="1"/>
       <c r="AD36" t="s">
-        <v>102</v>
+        <v>1</v>
       </c>
     </row>
     <row r="37" spans="21:30">
       <c r="U37" s="1" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="Y37" t="s">
         <v>0</v>
       </c>
+      <c r="AB37" s="1"/>
       <c r="AD37" t="s">
-        <v>102</v>
+        <v>1</v>
       </c>
     </row>
     <row r="38" spans="21:30">
       <c r="U38" s="1" t="s">
-        <v>110</v>
+        <v>25</v>
       </c>
       <c r="Y38" t="s">
         <v>0</v>
       </c>
+      <c r="AB38" s="1"/>
     </row>
     <row r="39" spans="21:30">
       <c r="U39" s="1" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="Y39" t="s">
         <v>0</v>
       </c>
+      <c r="AB39" s="1"/>
     </row>
     <row r="40" spans="21:30">
       <c r="U40" s="1" t="s">
-        <v>22</v>
+        <v>82</v>
       </c>
       <c r="Y40" t="s">
         <v>0</v>
       </c>
+      <c r="AB40" s="1"/>
     </row>
     <row r="41" spans="21:30">
       <c r="U41" s="1" t="s">
-        <v>23</v>
+        <v>61</v>
       </c>
       <c r="Y41" t="s">
         <v>0</v>
       </c>
+      <c r="AB41" s="1"/>
     </row>
     <row r="42" spans="21:30">
       <c r="U42" s="1" t="s">
-        <v>111</v>
+        <v>77</v>
       </c>
       <c r="Y42" t="s">
         <v>0</v>
       </c>
+      <c r="AB42" s="1"/>
     </row>
     <row r="43" spans="21:30">
       <c r="U43" s="1" t="s">
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="Y43" t="s">
         <v>0</v>
       </c>
+      <c r="AB43" s="1"/>
     </row>
     <row r="44" spans="21:30">
       <c r="U44" s="1" t="s">
-        <v>112</v>
+        <v>99</v>
       </c>
       <c r="Y44" t="s">
         <v>0</v>
       </c>
+      <c r="AB44" s="1"/>
     </row>
     <row r="45" spans="21:30">
       <c r="U45" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="Y45" t="s">
         <v>0</v>
       </c>
+      <c r="AB45" s="1"/>
     </row>
     <row r="46" spans="21:30">
       <c r="U46" s="1" t="s">
-        <v>26</v>
+        <v>78</v>
       </c>
       <c r="Y46" t="s">
         <v>0</v>
       </c>
+      <c r="AB46" s="1"/>
     </row>
     <row r="47" spans="21:30">
       <c r="U47" s="1" t="s">
-        <v>27</v>
+        <v>47</v>
       </c>
       <c r="Y47" t="s">
         <v>0</v>
       </c>
+      <c r="AB47" s="1"/>
     </row>
     <row r="48" spans="21:30">
       <c r="U48" s="1" t="s">
-        <v>113</v>
+        <v>65</v>
       </c>
       <c r="Y48" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="49" spans="21:25">
+      <c r="AB48" s="1"/>
+    </row>
+    <row r="49" spans="21:28">
       <c r="U49" s="1" t="s">
-        <v>99</v>
+        <v>27</v>
       </c>
       <c r="Y49" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="50" spans="21:25">
+      <c r="AB49" s="1"/>
+    </row>
+    <row r="50" spans="21:28">
       <c r="U50" s="1" t="s">
-        <v>114</v>
+        <v>66</v>
       </c>
       <c r="Y50" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="51" spans="21:25">
+      <c r="AB50" s="1"/>
+    </row>
+    <row r="51" spans="21:28">
       <c r="U51" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="Y51" t="s">
+        <v>0</v>
+      </c>
+      <c r="AB51" s="1"/>
+    </row>
+    <row r="52" spans="21:28">
+      <c r="U52" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="Y52" t="s">
+        <v>0</v>
+      </c>
+      <c r="AB52" s="1"/>
+    </row>
+    <row r="53" spans="21:28">
+      <c r="U53" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="Y53" t="s">
+        <v>0</v>
+      </c>
+      <c r="AB53" s="1"/>
+    </row>
+    <row r="54" spans="21:28">
+      <c r="U54" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="Y51" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="52" spans="21:25">
-      <c r="U52" s="1" t="s">
+      <c r="Y54" t="s">
+        <v>0</v>
+      </c>
+      <c r="AB54" s="1"/>
+    </row>
+    <row r="55" spans="21:28">
+      <c r="U55" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="Y55" t="s">
+        <v>0</v>
+      </c>
+      <c r="AB55" s="1"/>
+    </row>
+    <row r="56" spans="21:28">
+      <c r="U56" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="Y56" t="s">
+        <v>0</v>
+      </c>
+      <c r="AB56" s="1"/>
+    </row>
+    <row r="57" spans="21:28">
+      <c r="U57" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="Y57" t="s">
+        <v>0</v>
+      </c>
+      <c r="AB57" s="1"/>
+    </row>
+    <row r="58" spans="21:28">
+      <c r="U58" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="Y52" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="53" spans="21:25">
-      <c r="U53" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="Y53" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="54" spans="21:25">
-      <c r="U54" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="Y54" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="55" spans="21:25">
-      <c r="U55" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="Y55" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="56" spans="21:25">
-      <c r="U56" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="Y56" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="57" spans="21:25">
-      <c r="U57" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="Y57" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="58" spans="21:25">
-      <c r="U58" s="1" t="s">
-        <v>115</v>
-      </c>
       <c r="Y58" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="59" spans="21:25">
+      <c r="AB58" s="1"/>
+    </row>
+    <row r="59" spans="21:28">
       <c r="U59" s="1" t="s">
-        <v>116</v>
+        <v>76</v>
       </c>
       <c r="Y59" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="60" spans="21:25">
+      <c r="AB59" s="1"/>
+    </row>
+    <row r="60" spans="21:28">
       <c r="U60" s="1" t="s">
         <v>35</v>
       </c>
       <c r="Y60" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="61" spans="21:25">
+      <c r="AB60" s="1"/>
+    </row>
+    <row r="61" spans="21:28">
       <c r="U61" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="Y61" t="s">
+        <v>0</v>
+      </c>
+      <c r="AB61" s="1"/>
+    </row>
+    <row r="62" spans="21:28">
+      <c r="U62" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="Y62" t="s">
+        <v>0</v>
+      </c>
+      <c r="AB62" s="1"/>
+    </row>
+    <row r="63" spans="21:28">
+      <c r="U63" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="Y63" t="s">
+        <v>0</v>
+      </c>
+      <c r="AB63" s="1"/>
+    </row>
+    <row r="64" spans="21:28">
+      <c r="U64" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="Y61" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="62" spans="21:25">
-      <c r="U62" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="Y62" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="63" spans="21:25">
-      <c r="U63" s="1" t="s">
+      <c r="Y64" t="s">
+        <v>0</v>
+      </c>
+      <c r="AB64" s="1"/>
+    </row>
+    <row r="65" spans="21:28">
+      <c r="U65" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="Y65" t="s">
+        <v>0</v>
+      </c>
+      <c r="AB65" s="1"/>
+    </row>
+    <row r="66" spans="21:28">
+      <c r="U66" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="Y66" t="s">
+        <v>0</v>
+      </c>
+      <c r="AB66" s="1"/>
+    </row>
+    <row r="67" spans="21:28">
+      <c r="U67" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="Y67" t="s">
+        <v>0</v>
+      </c>
+      <c r="AB67" s="1"/>
+    </row>
+    <row r="68" spans="21:28">
+      <c r="U68" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="Y63" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="64" spans="21:25">
-      <c r="U64" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="Y64" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="65" spans="21:25">
-      <c r="U65" s="1" t="s">
+      <c r="Y68" t="s">
+        <v>0</v>
+      </c>
+      <c r="AB68" s="1"/>
+    </row>
+    <row r="69" spans="21:28">
+      <c r="U69" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="Y65" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="66" spans="21:25">
-      <c r="U66" s="1" t="s">
+      <c r="Y69" t="s">
+        <v>0</v>
+      </c>
+      <c r="AB69" s="1"/>
+    </row>
+    <row r="70" spans="21:28">
+      <c r="U70" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Y70" t="s">
+        <v>0</v>
+      </c>
+      <c r="AB70" s="1"/>
+    </row>
+    <row r="71" spans="21:28">
+      <c r="U71" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="Y66" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="67" spans="21:25">
-      <c r="U67" s="1" t="s">
+      <c r="Y71" t="s">
+        <v>0</v>
+      </c>
+      <c r="AB71" s="1"/>
+    </row>
+    <row r="72" spans="21:28">
+      <c r="U72" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="Y72" t="s">
+        <v>0</v>
+      </c>
+      <c r="AB72" s="1"/>
+    </row>
+    <row r="73" spans="21:28">
+      <c r="U73" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="Y73" t="s">
+        <v>0</v>
+      </c>
+      <c r="AB73" s="1"/>
+    </row>
+    <row r="74" spans="21:28">
+      <c r="U74" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="Y74" t="s">
+        <v>0</v>
+      </c>
+      <c r="AB74" s="1"/>
+    </row>
+    <row r="75" spans="21:28">
+      <c r="U75" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="Y75" t="s">
+        <v>0</v>
+      </c>
+      <c r="AB75" s="1"/>
+    </row>
+    <row r="76" spans="21:28">
+      <c r="U76" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="Y67" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="68" spans="21:25">
-      <c r="U68" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="Y68" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="69" spans="21:25">
-      <c r="U69" s="1" t="s">
+      <c r="Y76" t="s">
+        <v>0</v>
+      </c>
+      <c r="AB76" s="1"/>
+    </row>
+    <row r="77" spans="21:28">
+      <c r="U77" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="Y69" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="70" spans="21:25">
-      <c r="U70" s="1" t="s">
+      <c r="Y77" t="s">
+        <v>0</v>
+      </c>
+      <c r="AB77" s="1"/>
+    </row>
+    <row r="78" spans="21:28">
+      <c r="U78" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="Y78" t="s">
+        <v>0</v>
+      </c>
+      <c r="AB78" s="1"/>
+    </row>
+    <row r="79" spans="21:28">
+      <c r="U79" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="Y79" t="s">
+        <v>0</v>
+      </c>
+      <c r="AB79" s="1"/>
+    </row>
+    <row r="80" spans="21:28">
+      <c r="U80" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="Y80" t="s">
+        <v>0</v>
+      </c>
+      <c r="AB80" s="1"/>
+    </row>
+    <row r="81" spans="21:28">
+      <c r="U81" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="Y70" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="71" spans="21:25">
-      <c r="U71" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="Y71" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="72" spans="21:25">
-      <c r="U72" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="Y72" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="73" spans="21:25">
-      <c r="U73" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="Y73" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="74" spans="21:25">
-      <c r="U74" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="Y74" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="75" spans="21:25">
-      <c r="U75" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="Y75" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="76" spans="21:25">
-      <c r="U76" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="Y76" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="77" spans="21:25">
-      <c r="U77" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="Y77" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="78" spans="21:25">
-      <c r="U78" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="Y78" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="79" spans="21:25">
-      <c r="U79" s="1" t="s">
+      <c r="Y81" t="s">
+        <v>0</v>
+      </c>
+      <c r="AB81" s="1"/>
+    </row>
+    <row r="82" spans="21:28">
+      <c r="U82" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="Y82" t="s">
+        <v>0</v>
+      </c>
+      <c r="AB82" s="1"/>
+    </row>
+    <row r="83" spans="21:28">
+      <c r="U83" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="Y83" t="s">
+        <v>0</v>
+      </c>
+      <c r="AB83" s="1"/>
+    </row>
+    <row r="84" spans="21:28">
+      <c r="U84" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="Y84" t="s">
+        <v>0</v>
+      </c>
+      <c r="AB84" s="1"/>
+    </row>
+    <row r="85" spans="21:28">
+      <c r="U85" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="Y85" t="s">
+        <v>0</v>
+      </c>
+      <c r="AB85" s="1"/>
+    </row>
+    <row r="86" spans="21:28">
+      <c r="U86" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="Y86" t="s">
+        <v>0</v>
+      </c>
+      <c r="AB86" s="1"/>
+    </row>
+    <row r="87" spans="21:28">
+      <c r="U87" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="Y87" t="s">
+        <v>0</v>
+      </c>
+      <c r="AB87" s="1"/>
+    </row>
+    <row r="88" spans="21:28">
+      <c r="U88" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="Y88" t="s">
+        <v>0</v>
+      </c>
+      <c r="AB88" s="1"/>
+    </row>
+    <row r="89" spans="21:28">
+      <c r="U89" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="Y89" t="s">
+        <v>0</v>
+      </c>
+      <c r="AB89" s="1"/>
+    </row>
+    <row r="90" spans="21:28">
+      <c r="U90" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="Y90" t="s">
+        <v>0</v>
+      </c>
+      <c r="AB90" s="1"/>
+    </row>
+    <row r="91" spans="21:28">
+      <c r="U91" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="Y91" t="s">
+        <v>0</v>
+      </c>
+      <c r="AB91" s="1"/>
+    </row>
+    <row r="92" spans="21:28">
+      <c r="U92" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="Y92" t="s">
+        <v>0</v>
+      </c>
+      <c r="AB92" s="1"/>
+    </row>
+    <row r="93" spans="21:28">
+      <c r="U93" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="Y93" t="s">
+        <v>0</v>
+      </c>
+      <c r="AB93" s="1"/>
+    </row>
+    <row r="94" spans="21:28">
+      <c r="U94" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="Y94" t="s">
+        <v>0</v>
+      </c>
+      <c r="AB94" s="1"/>
+    </row>
+    <row r="95" spans="21:28">
+      <c r="U95" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="Y95" t="s">
+        <v>0</v>
+      </c>
+      <c r="AB95" s="1"/>
+    </row>
+    <row r="96" spans="21:28">
+      <c r="U96" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="Y79" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="80" spans="21:25">
-      <c r="U80" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="Y80" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="81" spans="21:25">
-      <c r="U81" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="Y81" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="82" spans="21:25">
-      <c r="U82" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="Y82" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="83" spans="21:25">
-      <c r="U83" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="Y83" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="84" spans="21:25">
-      <c r="U84" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="Y84" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="85" spans="21:25">
-      <c r="U85" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="Y85" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="86" spans="21:25">
-      <c r="U86" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="Y86" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="87" spans="21:25">
-      <c r="U87" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="Y87" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="88" spans="21:25">
-      <c r="U88" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="Y88" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="89" spans="21:25">
-      <c r="U89" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="Y89" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="90" spans="21:25">
-      <c r="U90" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="Y90" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="91" spans="21:25">
-      <c r="U91" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="Y91" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="92" spans="21:25">
-      <c r="U92" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="Y92" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="93" spans="21:25">
-      <c r="U93" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="Y93" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="94" spans="21:25">
-      <c r="U94" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="Y94" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="95" spans="21:25">
-      <c r="U95" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="Y95" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="96" spans="21:25">
-      <c r="U96" s="1" t="s">
-        <v>125</v>
-      </c>
       <c r="Y96" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="97" spans="21:25">
+      <c r="AB96" s="1"/>
+    </row>
+    <row r="97" spans="21:28">
       <c r="U97" s="1" t="s">
-        <v>62</v>
+        <v>80</v>
       </c>
       <c r="Y97" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="98" spans="21:25">
+      <c r="AB97" s="1"/>
+    </row>
+    <row r="98" spans="21:28">
       <c r="U98" s="1" t="s">
-        <v>126</v>
+        <v>13</v>
       </c>
       <c r="Y98" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="99" spans="21:25">
-      <c r="U99" s="1" t="s">
-        <v>64</v>
-      </c>
+      <c r="AB98" s="1"/>
+    </row>
+    <row r="99" spans="21:28">
+      <c r="U99" s="1"/>
       <c r="Y99" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="100" spans="21:25">
-      <c r="U100" s="1" t="s">
-        <v>63</v>
-      </c>
+      <c r="AB99" s="1"/>
+    </row>
+    <row r="100" spans="21:28">
+      <c r="U100" s="1"/>
       <c r="Y100" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="101" spans="21:25">
-      <c r="U101" s="1" t="s">
-        <v>65</v>
-      </c>
+      <c r="AB100" s="1"/>
+    </row>
+    <row r="101" spans="21:28">
+      <c r="U101" s="1"/>
       <c r="Y101" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="102" spans="21:25">
-      <c r="U102" s="1" t="s">
-        <v>127</v>
-      </c>
+      <c r="AB101" s="1"/>
+    </row>
+    <row r="102" spans="21:28">
+      <c r="U102" s="1"/>
       <c r="Y102" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="103" spans="21:25">
-      <c r="U103" s="1" t="s">
-        <v>66</v>
-      </c>
+      <c r="AB102" s="1"/>
+    </row>
+    <row r="103" spans="21:28">
+      <c r="U103" s="1"/>
       <c r="Y103" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="104" spans="21:25">
-      <c r="U104" s="1" t="s">
-        <v>67</v>
-      </c>
+      <c r="AB103" s="1"/>
+    </row>
+    <row r="104" spans="21:28">
+      <c r="U104" s="1"/>
       <c r="Y104" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="105" spans="21:25">
-      <c r="U105" s="1" t="s">
-        <v>68</v>
-      </c>
+      <c r="AB104" s="1"/>
+    </row>
+    <row r="105" spans="21:28">
+      <c r="U105" s="1"/>
       <c r="Y105" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="106" spans="21:25">
-      <c r="U106" s="1" t="s">
-        <v>69</v>
-      </c>
+      <c r="AB105" s="1"/>
+    </row>
+    <row r="106" spans="21:28">
+      <c r="U106" s="1"/>
       <c r="Y106" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="107" spans="21:25">
-      <c r="U107" s="1" t="s">
-        <v>128</v>
-      </c>
+      <c r="AB106" s="1"/>
+    </row>
+    <row r="107" spans="21:28">
+      <c r="U107" s="1"/>
       <c r="Y107" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="108" spans="21:25">
-      <c r="U108" s="1" t="s">
-        <v>70</v>
-      </c>
+      <c r="AB107" s="1"/>
+    </row>
+    <row r="108" spans="21:28">
+      <c r="U108" s="1"/>
       <c r="Y108" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="109" spans="21:25">
-      <c r="U109" s="1" t="s">
-        <v>71</v>
-      </c>
+      <c r="AB108" s="1"/>
+    </row>
+    <row r="109" spans="21:28">
+      <c r="U109" s="1"/>
       <c r="Y109" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="110" spans="21:25">
-      <c r="U110" s="1" t="s">
-        <v>129</v>
-      </c>
+      <c r="AB109" s="1"/>
+    </row>
+    <row r="110" spans="21:28">
+      <c r="U110" s="1"/>
       <c r="Y110" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="111" spans="21:25">
-      <c r="U111" s="1" t="s">
-        <v>73</v>
-      </c>
+      <c r="AB110" s="1"/>
+    </row>
+    <row r="111" spans="21:28">
+      <c r="U111" s="1"/>
       <c r="Y111" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="112" spans="21:25">
-      <c r="U112" s="1" t="s">
-        <v>72</v>
-      </c>
+      <c r="AB111" s="1"/>
+    </row>
+    <row r="112" spans="21:28">
+      <c r="U112" s="1"/>
       <c r="Y112" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="113" spans="21:25">
-      <c r="U113" s="1" t="s">
-        <v>74</v>
-      </c>
+      <c r="AB112" s="1"/>
+    </row>
+    <row r="113" spans="21:28">
+      <c r="U113" s="1"/>
       <c r="Y113" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="114" spans="21:25">
-      <c r="U114" s="1" t="s">
-        <v>75</v>
-      </c>
+      <c r="AB113" s="1"/>
+    </row>
+    <row r="114" spans="21:28">
+      <c r="U114" s="1"/>
       <c r="Y114" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="115" spans="21:25">
-      <c r="U115" s="1" t="s">
-        <v>130</v>
-      </c>
+      <c r="AB114" s="1"/>
+    </row>
+    <row r="115" spans="21:28">
+      <c r="U115" s="1"/>
       <c r="Y115" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="116" spans="21:25">
-      <c r="U116" s="1" t="s">
-        <v>76</v>
-      </c>
+      <c r="AB115" s="1"/>
+    </row>
+    <row r="116" spans="21:28">
+      <c r="U116" s="1"/>
       <c r="Y116" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="117" spans="21:25">
-      <c r="U117" s="1" t="s">
-        <v>131</v>
-      </c>
+    <row r="117" spans="21:28">
+      <c r="U117" s="1"/>
       <c r="Y117" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="118" spans="21:25">
-      <c r="U118" s="1" t="s">
-        <v>77</v>
-      </c>
+    <row r="118" spans="21:28">
+      <c r="U118" s="1"/>
       <c r="Y118" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="119" spans="21:25">
-      <c r="U119" s="1" t="s">
-        <v>132</v>
-      </c>
+    <row r="119" spans="21:28">
+      <c r="U119" s="1"/>
       <c r="Y119" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="120" spans="21:25">
-      <c r="U120" s="1" t="s">
-        <v>78</v>
-      </c>
+    <row r="120" spans="21:28">
+      <c r="U120" s="1"/>
       <c r="Y120" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="121" spans="21:25">
-      <c r="U121" s="1" t="s">
-        <v>79</v>
-      </c>
+    <row r="121" spans="21:28">
+      <c r="U121" s="1"/>
       <c r="Y121" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="122" spans="21:25">
-      <c r="U122" s="1" t="s">
-        <v>80</v>
-      </c>
+    <row r="122" spans="21:28">
+      <c r="U122" s="1"/>
       <c r="Y122" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="123" spans="21:25">
-      <c r="U123" s="1" t="s">
-        <v>92</v>
-      </c>
+    <row r="123" spans="21:28">
+      <c r="U123" s="1"/>
       <c r="Y123" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="124" spans="21:25">
-      <c r="U124" s="1" t="s">
-        <v>138</v>
-      </c>
+    <row r="124" spans="21:28">
+      <c r="U124" s="1"/>
       <c r="Y124" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="125" spans="21:25">
-      <c r="U125" s="1" t="s">
-        <v>81</v>
-      </c>
+    <row r="125" spans="21:28">
+      <c r="U125" s="1"/>
       <c r="Y125" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="126" spans="21:25">
-      <c r="U126" s="1" t="s">
-        <v>82</v>
-      </c>
+    <row r="126" spans="21:28">
+      <c r="U126" s="1"/>
       <c r="Y126" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="127" spans="21:25">
-      <c r="U127" s="1" t="s">
-        <v>83</v>
-      </c>
+    <row r="127" spans="21:28">
+      <c r="U127" s="1"/>
       <c r="Y127" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="128" spans="21:25">
-      <c r="U128" s="1" t="s">
-        <v>84</v>
-      </c>
+    <row r="128" spans="21:28">
+      <c r="U128" s="1"/>
       <c r="Y128" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="129" spans="21:25">
-      <c r="U129" s="1" t="s">
-        <v>100</v>
-      </c>
+      <c r="U129" s="1"/>
       <c r="Y129" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="130" spans="21:25">
-      <c r="U130" s="1" t="s">
-        <v>85</v>
-      </c>
+      <c r="U130" s="1"/>
       <c r="Y130" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="131" spans="21:25">
-      <c r="U131" s="1" t="s">
-        <v>86</v>
-      </c>
+      <c r="U131" s="1"/>
       <c r="Y131" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="132" spans="21:25">
-      <c r="U132" s="1" t="s">
-        <v>88</v>
-      </c>
+      <c r="U132" s="1"/>
       <c r="Y132" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="133" spans="21:25">
-      <c r="U133" s="1" t="s">
-        <v>87</v>
-      </c>
+      <c r="U133" s="1"/>
       <c r="Y133" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="134" spans="21:25">
-      <c r="U134" s="1" t="s">
-        <v>89</v>
-      </c>
+      <c r="U134" s="1"/>
       <c r="Y134" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="135" spans="21:25">
-      <c r="U135" s="1" t="s">
-        <v>133</v>
-      </c>
+      <c r="U135" s="1"/>
       <c r="Y135" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="136" spans="21:25">
-      <c r="U136" s="1" t="s">
-        <v>90</v>
-      </c>
+      <c r="U136" s="1"/>
       <c r="Y136" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="137" spans="21:25">
-      <c r="U137" s="1" t="s">
-        <v>101</v>
-      </c>
+      <c r="U137" s="1"/>
       <c r="Y137" t="s">
         <v>0</v>
       </c>
@@ -4481,16 +4342,16 @@
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B6:Q21">
-    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
+  <conditionalFormatting sqref="R6:R7 B6:Q21">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
+      <formula>"p"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>"o"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="0" priority="3" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
-      <formula>"p"</formula>
-    </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>